<commit_message>
Update SRS and Layout Design
</commit_message>
<xml_diff>
--- a/doc/design/layout/EnglishSound_Design.xlsx
+++ b/doc/design/layout/EnglishSound_Design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Github\word-of-the-day\doc\design\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE8655E-8CE2-4E2C-B405-61EA94934FC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D956A572-3F2F-4260-8D54-1315321992F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="Hộp_thoại_tìm_và_nạp_khách_hàng_có_sẵn">#REF!</definedName>
     <definedName name="Màn_hình_thêm_thiết_bị__thiết_bị_này_do_đối_tác_bên_ngoài_cung_cấp">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Layout_Menu!$A$1:$BA$131</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Layout_Menu!$A$1:$BA$175</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Record of change'!$A$1:$E$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Template!$A$1:$AJ$38</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Layout_Menu!$1:$4</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
   <si>
     <r>
       <t>*A - Add</t>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>The first version</t>
@@ -191,9 +188,6 @@
   </si>
   <si>
     <t>Sign in</t>
-  </si>
-  <si>
-    <t>10/12/2018</t>
   </si>
   <si>
     <t>Dictionary</t>
@@ -328,10 +322,37 @@
     <t>3. Sign In and Sign up form</t>
   </si>
   <si>
-    <t>20/12/2018</t>
+    <t>Quan.N.C.T</t>
   </si>
   <si>
-    <t>Quan.N.C.T</t>
+    <t>4. Upload Page</t>
+  </si>
+  <si>
+    <t>WORD:</t>
+  </si>
+  <si>
+    <t>Enter word…</t>
+  </si>
+  <si>
+    <t>EXPLAIN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter word description link or directory </t>
+  </si>
+  <si>
+    <t>AUDIO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter audio link or directory </t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>25/12/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the upload page </t>
   </si>
 </sst>
 </file>
@@ -2171,7 +2192,7 @@
     <xf numFmtId="0" fontId="13" fillId="20" borderId="67" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="68" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="37" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2390,52 +2411,13 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="80" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="81" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="52" fillId="30" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="71" fillId="32" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="32" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="32" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="32" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="32" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="32" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="32" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="32" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="32" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="32" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="32" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="24" xfId="38" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="29" borderId="24" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="29" borderId="26" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2528,10 +2510,49 @@
     <xf numFmtId="14" fontId="18" fillId="0" borderId="24" xfId="38" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="24" xfId="38" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="24" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="32" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="32" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="32" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="32" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="32" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="32" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="32" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="32" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="32" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="32" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="32" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="27" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2723,6 +2744,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="78" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2808,8 +2834,8 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FF00CC00"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF0000CC"/>
       <color rgb="FF000099"/>
       <color rgb="FFFF33CC"/>
@@ -3224,6 +3250,67 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>33867</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{141A4F09-8B08-46CB-990D-7950F426CCCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="177800" y="25476200"/>
+          <a:ext cx="440267" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3618,17 +3705,17 @@
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1">
       <c r="A5" s="76" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3644,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AZ131"/>
+  <dimension ref="A1:AZ164"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="AY9" sqref="AY9"/>
+      <selection activeCell="D1" sqref="D1:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.88671875" defaultRowHeight="13.8"/>
@@ -3674,236 +3761,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="12.15" customHeight="1">
-      <c r="A1" s="176" t="s">
-        <v>25</v>
+      <c r="A1" s="163" t="s">
+        <v>24</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="180" t="s">
-        <v>34</v>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="167" t="s">
+        <v>33</v>
       </c>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
-      <c r="AF1" s="184" t="s">
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="167"/>
+      <c r="AB1" s="167"/>
+      <c r="AC1" s="167"/>
+      <c r="AD1" s="167"/>
+      <c r="AE1" s="167"/>
+      <c r="AF1" s="171" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG1" s="172"/>
+      <c r="AH1" s="172"/>
+      <c r="AI1" s="172"/>
+      <c r="AJ1" s="172"/>
+      <c r="AK1" s="172"/>
+      <c r="AL1" s="172"/>
+      <c r="AM1" s="172"/>
+      <c r="AN1" s="172"/>
+      <c r="AO1" s="172"/>
+      <c r="AP1" s="172"/>
+      <c r="AQ1" s="172"/>
+      <c r="AR1" s="172"/>
+      <c r="AS1" s="172"/>
+      <c r="AT1" s="172"/>
+      <c r="AU1" s="172"/>
+      <c r="AV1" s="173"/>
+    </row>
+    <row r="2" spans="1:52" ht="14.1" customHeight="1">
+      <c r="A2" s="165"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
+      <c r="K2" s="168"/>
+      <c r="L2" s="168"/>
+      <c r="M2" s="168"/>
+      <c r="N2" s="168"/>
+      <c r="O2" s="168"/>
+      <c r="P2" s="168"/>
+      <c r="Q2" s="168"/>
+      <c r="R2" s="168"/>
+      <c r="S2" s="168"/>
+      <c r="T2" s="168"/>
+      <c r="U2" s="168"/>
+      <c r="V2" s="168"/>
+      <c r="W2" s="168"/>
+      <c r="X2" s="168"/>
+      <c r="Y2" s="168"/>
+      <c r="Z2" s="168"/>
+      <c r="AA2" s="168"/>
+      <c r="AB2" s="168"/>
+      <c r="AC2" s="168"/>
+      <c r="AD2" s="168"/>
+      <c r="AE2" s="168"/>
+      <c r="AF2" s="174" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="185"/>
-      <c r="AH1" s="185"/>
-      <c r="AI1" s="185"/>
-      <c r="AJ1" s="185"/>
-      <c r="AK1" s="185"/>
-      <c r="AL1" s="185"/>
-      <c r="AM1" s="185"/>
-      <c r="AN1" s="185"/>
-      <c r="AO1" s="185"/>
-      <c r="AP1" s="185"/>
-      <c r="AQ1" s="185"/>
-      <c r="AR1" s="185"/>
-      <c r="AS1" s="185"/>
-      <c r="AT1" s="185"/>
-      <c r="AU1" s="185"/>
-      <c r="AV1" s="186"/>
-    </row>
-    <row r="2" spans="1:52" ht="14.1" customHeight="1">
-      <c r="A2" s="178"/>
-      <c r="B2" s="179"/>
-      <c r="C2" s="179"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="181"/>
-      <c r="G2" s="181"/>
-      <c r="H2" s="181"/>
-      <c r="I2" s="181"/>
-      <c r="J2" s="181"/>
-      <c r="K2" s="181"/>
-      <c r="L2" s="181"/>
-      <c r="M2" s="181"/>
-      <c r="N2" s="181"/>
-      <c r="O2" s="181"/>
-      <c r="P2" s="181"/>
-      <c r="Q2" s="181"/>
-      <c r="R2" s="181"/>
-      <c r="S2" s="181"/>
-      <c r="T2" s="181"/>
-      <c r="U2" s="181"/>
-      <c r="V2" s="181"/>
-      <c r="W2" s="181"/>
-      <c r="X2" s="181"/>
-      <c r="Y2" s="181"/>
-      <c r="Z2" s="181"/>
-      <c r="AA2" s="181"/>
-      <c r="AB2" s="181"/>
-      <c r="AC2" s="181"/>
-      <c r="AD2" s="181"/>
-      <c r="AE2" s="181"/>
-      <c r="AF2" s="187" t="s">
+      <c r="AG2" s="175"/>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="175"/>
+      <c r="AK2" s="175"/>
+      <c r="AL2" s="175"/>
+      <c r="AM2" s="175"/>
+      <c r="AN2" s="175"/>
+      <c r="AO2" s="175"/>
+      <c r="AP2" s="175"/>
+      <c r="AQ2" s="175"/>
+      <c r="AR2" s="175"/>
+      <c r="AS2" s="175"/>
+      <c r="AT2" s="175"/>
+      <c r="AU2" s="175"/>
+      <c r="AV2" s="176"/>
+    </row>
+    <row r="3" spans="1:52">
+      <c r="A3" s="177" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="183" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="185"/>
+      <c r="L3" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" s="188"/>
-      <c r="AH2" s="188"/>
-      <c r="AI2" s="188"/>
-      <c r="AJ2" s="188"/>
-      <c r="AK2" s="188"/>
-      <c r="AL2" s="188"/>
-      <c r="AM2" s="188"/>
-      <c r="AN2" s="188"/>
-      <c r="AO2" s="188"/>
-      <c r="AP2" s="188"/>
-      <c r="AQ2" s="188"/>
-      <c r="AR2" s="188"/>
-      <c r="AS2" s="188"/>
-      <c r="AT2" s="188"/>
-      <c r="AU2" s="188"/>
-      <c r="AV2" s="189"/>
-    </row>
-    <row r="3" spans="1:52">
-      <c r="A3" s="190" t="s">
+      <c r="M3" s="178"/>
+      <c r="N3" s="178"/>
+      <c r="O3" s="178"/>
+      <c r="P3" s="178"/>
+      <c r="Q3" s="179"/>
+      <c r="R3" s="183" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="184"/>
+      <c r="T3" s="184"/>
+      <c r="U3" s="184"/>
+      <c r="V3" s="184"/>
+      <c r="W3" s="184"/>
+      <c r="X3" s="184"/>
+      <c r="Y3" s="184"/>
+      <c r="Z3" s="184"/>
+      <c r="AA3" s="184"/>
+      <c r="AB3" s="184"/>
+      <c r="AC3" s="184"/>
+      <c r="AD3" s="184"/>
+      <c r="AE3" s="185"/>
+      <c r="AF3" s="191" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG3" s="191"/>
+      <c r="AH3" s="191"/>
+      <c r="AI3" s="191"/>
+      <c r="AJ3" s="191"/>
+      <c r="AK3" s="192" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL3" s="193"/>
+      <c r="AM3" s="193"/>
+      <c r="AN3" s="193"/>
+      <c r="AO3" s="191" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP3" s="191"/>
+      <c r="AQ3" s="191"/>
+      <c r="AR3" s="191"/>
+      <c r="AS3" s="194" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT3" s="194"/>
+      <c r="AU3" s="194"/>
+      <c r="AV3" s="195"/>
+    </row>
+    <row r="4" spans="1:52">
+      <c r="A4" s="180"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="188"/>
+      <c r="L4" s="190"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="181"/>
+      <c r="O4" s="181"/>
+      <c r="P4" s="181"/>
+      <c r="Q4" s="182"/>
+      <c r="R4" s="186"/>
+      <c r="S4" s="187"/>
+      <c r="T4" s="187"/>
+      <c r="U4" s="187"/>
+      <c r="V4" s="187"/>
+      <c r="W4" s="187"/>
+      <c r="X4" s="187"/>
+      <c r="Y4" s="187"/>
+      <c r="Z4" s="187"/>
+      <c r="AA4" s="187"/>
+      <c r="AB4" s="187"/>
+      <c r="AC4" s="187"/>
+      <c r="AD4" s="187"/>
+      <c r="AE4" s="188"/>
+      <c r="AF4" s="196" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="196" t="s">
-        <v>19</v>
+      <c r="AG4" s="196"/>
+      <c r="AH4" s="196"/>
+      <c r="AI4" s="196"/>
+      <c r="AJ4" s="196"/>
+      <c r="AK4" s="192" t="s">
+        <v>88</v>
       </c>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
-      <c r="I3" s="197"/>
-      <c r="J3" s="197"/>
-      <c r="K3" s="198"/>
-      <c r="L3" s="202" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="191"/>
-      <c r="N3" s="191"/>
-      <c r="O3" s="191"/>
-      <c r="P3" s="191"/>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="196" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" s="197"/>
-      <c r="T3" s="197"/>
-      <c r="U3" s="197"/>
-      <c r="V3" s="197"/>
-      <c r="W3" s="197"/>
-      <c r="X3" s="197"/>
-      <c r="Y3" s="197"/>
-      <c r="Z3" s="197"/>
-      <c r="AA3" s="197"/>
-      <c r="AB3" s="197"/>
-      <c r="AC3" s="197"/>
-      <c r="AD3" s="197"/>
-      <c r="AE3" s="198"/>
-      <c r="AF3" s="204" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG3" s="204"/>
-      <c r="AH3" s="204"/>
-      <c r="AI3" s="204"/>
-      <c r="AJ3" s="204"/>
-      <c r="AK3" s="205" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL3" s="172"/>
-      <c r="AM3" s="172"/>
-      <c r="AN3" s="172"/>
-      <c r="AO3" s="204" t="s">
-        <v>10</v>
-      </c>
-      <c r="AP3" s="204"/>
-      <c r="AQ3" s="204"/>
-      <c r="AR3" s="204"/>
-      <c r="AS3" s="206" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT3" s="206"/>
-      <c r="AU3" s="206"/>
-      <c r="AV3" s="207"/>
-    </row>
-    <row r="4" spans="1:52">
-      <c r="A4" s="193"/>
-      <c r="B4" s="194"/>
-      <c r="C4" s="194"/>
-      <c r="D4" s="194"/>
-      <c r="E4" s="195"/>
-      <c r="F4" s="199"/>
-      <c r="G4" s="200"/>
-      <c r="H4" s="200"/>
-      <c r="I4" s="200"/>
-      <c r="J4" s="200"/>
-      <c r="K4" s="201"/>
-      <c r="L4" s="203"/>
-      <c r="M4" s="194"/>
-      <c r="N4" s="194"/>
-      <c r="O4" s="194"/>
-      <c r="P4" s="194"/>
-      <c r="Q4" s="195"/>
-      <c r="R4" s="199"/>
-      <c r="S4" s="200"/>
-      <c r="T4" s="200"/>
-      <c r="U4" s="200"/>
-      <c r="V4" s="200"/>
-      <c r="W4" s="200"/>
-      <c r="X4" s="200"/>
-      <c r="Y4" s="200"/>
-      <c r="Z4" s="200"/>
-      <c r="AA4" s="200"/>
-      <c r="AB4" s="200"/>
-      <c r="AC4" s="200"/>
-      <c r="AD4" s="200"/>
-      <c r="AE4" s="201"/>
-      <c r="AF4" s="173" t="s">
+      <c r="AL4" s="193"/>
+      <c r="AM4" s="193"/>
+      <c r="AN4" s="193"/>
+      <c r="AO4" s="196" t="s">
         <v>12</v>
       </c>
-      <c r="AG4" s="173"/>
-      <c r="AH4" s="173"/>
-      <c r="AI4" s="173"/>
-      <c r="AJ4" s="173"/>
-      <c r="AK4" s="205" t="s">
-        <v>81</v>
+      <c r="AP4" s="196"/>
+      <c r="AQ4" s="196"/>
+      <c r="AR4" s="196"/>
+      <c r="AS4" s="160" t="s">
+        <v>79</v>
       </c>
-      <c r="AL4" s="172"/>
-      <c r="AM4" s="172"/>
-      <c r="AN4" s="172"/>
-      <c r="AO4" s="173" t="s">
-        <v>13</v>
-      </c>
-      <c r="AP4" s="173"/>
-      <c r="AQ4" s="173"/>
-      <c r="AR4" s="173"/>
-      <c r="AS4" s="174" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT4" s="174"/>
-      <c r="AU4" s="174"/>
-      <c r="AV4" s="175"/>
+      <c r="AT4" s="160"/>
+      <c r="AU4" s="160"/>
+      <c r="AV4" s="161"/>
     </row>
     <row r="5" spans="1:52">
       <c r="A5" s="6"/>
@@ -3957,7 +4044,7 @@
     </row>
     <row r="6" spans="1:52">
       <c r="A6" s="67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -4060,7 +4147,7 @@
     <row r="8" spans="1:52">
       <c r="A8" s="11"/>
       <c r="B8" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -4112,7 +4199,7 @@
     <row r="9" spans="1:52">
       <c r="A9" s="11"/>
       <c r="B9" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -4164,7 +4251,7 @@
     <row r="10" spans="1:52">
       <c r="A10" s="11"/>
       <c r="B10" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="12"/>
@@ -4315,7 +4402,7 @@
     </row>
     <row r="13" spans="1:52">
       <c r="A13" s="67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="70"/>
       <c r="C13" s="70"/>
@@ -4368,7 +4455,7 @@
     <row r="14" spans="1:52">
       <c r="A14" s="64"/>
       <c r="B14" s="65" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="61"/>
       <c r="D14" s="61"/>
@@ -4421,7 +4508,7 @@
       <c r="A15" s="59"/>
       <c r="B15" s="60"/>
       <c r="C15" s="59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
@@ -4529,7 +4616,7 @@
       <c r="C17" s="99"/>
       <c r="D17" s="100"/>
       <c r="E17" s="117" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F17" s="101"/>
       <c r="G17" s="101"/>
@@ -4538,34 +4625,34 @@
       <c r="J17" s="101"/>
       <c r="K17" s="101"/>
       <c r="L17" s="116" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M17" s="100"/>
       <c r="N17" s="100"/>
       <c r="O17" s="99"/>
       <c r="P17" s="99"/>
       <c r="Q17" s="116" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R17" s="99"/>
       <c r="S17" s="99"/>
       <c r="T17" s="99"/>
       <c r="U17" s="99"/>
       <c r="V17" s="116" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W17" s="99"/>
       <c r="X17" s="99"/>
       <c r="Y17" s="99"/>
       <c r="Z17" s="116" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AA17" s="99"/>
       <c r="AB17" s="99"/>
       <c r="AC17" s="99"/>
       <c r="AD17" s="114"/>
       <c r="AE17" s="116" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AF17" s="99"/>
       <c r="AG17" s="99"/>
@@ -4574,21 +4661,21 @@
       <c r="AJ17" s="114"/>
       <c r="AK17" s="99"/>
       <c r="AL17" s="116" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AM17" s="102"/>
       <c r="AN17" s="99"/>
       <c r="AO17" s="99"/>
       <c r="AP17" s="99"/>
       <c r="AQ17" s="115" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AR17" s="99"/>
       <c r="AS17" s="99"/>
       <c r="AT17" s="99"/>
       <c r="AU17" s="99"/>
       <c r="AV17" s="116" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AW17" s="113"/>
       <c r="AX17" s="99"/>
@@ -4823,37 +4910,37 @@
       <c r="I22" s="57"/>
       <c r="J22" s="57"/>
       <c r="K22" s="57"/>
-      <c r="L22" s="182" t="s">
-        <v>43</v>
+      <c r="L22" s="169" t="s">
+        <v>41</v>
       </c>
-      <c r="M22" s="183"/>
-      <c r="N22" s="183"/>
-      <c r="O22" s="183"/>
-      <c r="P22" s="183"/>
-      <c r="Q22" s="183"/>
-      <c r="R22" s="183"/>
-      <c r="S22" s="183"/>
-      <c r="T22" s="183"/>
-      <c r="U22" s="183"/>
-      <c r="V22" s="183"/>
-      <c r="W22" s="183"/>
-      <c r="X22" s="183"/>
-      <c r="Y22" s="183"/>
-      <c r="Z22" s="183"/>
-      <c r="AA22" s="183"/>
-      <c r="AB22" s="183"/>
-      <c r="AC22" s="183"/>
-      <c r="AD22" s="183"/>
-      <c r="AE22" s="183"/>
-      <c r="AF22" s="183"/>
-      <c r="AG22" s="183"/>
-      <c r="AH22" s="183"/>
-      <c r="AI22" s="183"/>
-      <c r="AJ22" s="183"/>
-      <c r="AK22" s="183"/>
-      <c r="AL22" s="183"/>
-      <c r="AM22" s="183"/>
-      <c r="AN22" s="183"/>
+      <c r="M22" s="170"/>
+      <c r="N22" s="170"/>
+      <c r="O22" s="170"/>
+      <c r="P22" s="170"/>
+      <c r="Q22" s="170"/>
+      <c r="R22" s="170"/>
+      <c r="S22" s="170"/>
+      <c r="T22" s="170"/>
+      <c r="U22" s="170"/>
+      <c r="V22" s="170"/>
+      <c r="W22" s="170"/>
+      <c r="X22" s="170"/>
+      <c r="Y22" s="170"/>
+      <c r="Z22" s="170"/>
+      <c r="AA22" s="170"/>
+      <c r="AB22" s="170"/>
+      <c r="AC22" s="170"/>
+      <c r="AD22" s="170"/>
+      <c r="AE22" s="170"/>
+      <c r="AF22" s="170"/>
+      <c r="AG22" s="170"/>
+      <c r="AH22" s="170"/>
+      <c r="AI22" s="170"/>
+      <c r="AJ22" s="170"/>
+      <c r="AK22" s="170"/>
+      <c r="AL22" s="170"/>
+      <c r="AM22" s="170"/>
+      <c r="AN22" s="170"/>
       <c r="AO22" s="57"/>
       <c r="AP22" s="57"/>
       <c r="AQ22" s="57"/>
@@ -4879,35 +4966,35 @@
       <c r="I23" s="57"/>
       <c r="J23" s="72"/>
       <c r="K23" s="57"/>
-      <c r="L23" s="183"/>
-      <c r="M23" s="183"/>
-      <c r="N23" s="183"/>
-      <c r="O23" s="183"/>
-      <c r="P23" s="183"/>
-      <c r="Q23" s="183"/>
-      <c r="R23" s="183"/>
-      <c r="S23" s="183"/>
-      <c r="T23" s="183"/>
-      <c r="U23" s="183"/>
-      <c r="V23" s="183"/>
-      <c r="W23" s="183"/>
-      <c r="X23" s="183"/>
-      <c r="Y23" s="183"/>
-      <c r="Z23" s="183"/>
-      <c r="AA23" s="183"/>
-      <c r="AB23" s="183"/>
-      <c r="AC23" s="183"/>
-      <c r="AD23" s="183"/>
-      <c r="AE23" s="183"/>
-      <c r="AF23" s="183"/>
-      <c r="AG23" s="183"/>
-      <c r="AH23" s="183"/>
-      <c r="AI23" s="183"/>
-      <c r="AJ23" s="183"/>
-      <c r="AK23" s="183"/>
-      <c r="AL23" s="183"/>
-      <c r="AM23" s="183"/>
-      <c r="AN23" s="183"/>
+      <c r="L23" s="170"/>
+      <c r="M23" s="170"/>
+      <c r="N23" s="170"/>
+      <c r="O23" s="170"/>
+      <c r="P23" s="170"/>
+      <c r="Q23" s="170"/>
+      <c r="R23" s="170"/>
+      <c r="S23" s="170"/>
+      <c r="T23" s="170"/>
+      <c r="U23" s="170"/>
+      <c r="V23" s="170"/>
+      <c r="W23" s="170"/>
+      <c r="X23" s="170"/>
+      <c r="Y23" s="170"/>
+      <c r="Z23" s="170"/>
+      <c r="AA23" s="170"/>
+      <c r="AB23" s="170"/>
+      <c r="AC23" s="170"/>
+      <c r="AD23" s="170"/>
+      <c r="AE23" s="170"/>
+      <c r="AF23" s="170"/>
+      <c r="AG23" s="170"/>
+      <c r="AH23" s="170"/>
+      <c r="AI23" s="170"/>
+      <c r="AJ23" s="170"/>
+      <c r="AK23" s="170"/>
+      <c r="AL23" s="170"/>
+      <c r="AM23" s="170"/>
+      <c r="AN23" s="170"/>
       <c r="AO23" s="57"/>
       <c r="AP23" s="57"/>
       <c r="AQ23" s="57"/>
@@ -4933,35 +5020,35 @@
       <c r="I24" s="57"/>
       <c r="J24" s="57"/>
       <c r="K24" s="57"/>
-      <c r="L24" s="183"/>
-      <c r="M24" s="183"/>
-      <c r="N24" s="183"/>
-      <c r="O24" s="183"/>
-      <c r="P24" s="183"/>
-      <c r="Q24" s="183"/>
-      <c r="R24" s="183"/>
-      <c r="S24" s="183"/>
-      <c r="T24" s="183"/>
-      <c r="U24" s="183"/>
-      <c r="V24" s="183"/>
-      <c r="W24" s="183"/>
-      <c r="X24" s="183"/>
-      <c r="Y24" s="183"/>
-      <c r="Z24" s="183"/>
-      <c r="AA24" s="183"/>
-      <c r="AB24" s="183"/>
-      <c r="AC24" s="183"/>
-      <c r="AD24" s="183"/>
-      <c r="AE24" s="183"/>
-      <c r="AF24" s="183"/>
-      <c r="AG24" s="183"/>
-      <c r="AH24" s="183"/>
-      <c r="AI24" s="183"/>
-      <c r="AJ24" s="183"/>
-      <c r="AK24" s="183"/>
-      <c r="AL24" s="183"/>
-      <c r="AM24" s="183"/>
-      <c r="AN24" s="183"/>
+      <c r="L24" s="170"/>
+      <c r="M24" s="170"/>
+      <c r="N24" s="170"/>
+      <c r="O24" s="170"/>
+      <c r="P24" s="170"/>
+      <c r="Q24" s="170"/>
+      <c r="R24" s="170"/>
+      <c r="S24" s="170"/>
+      <c r="T24" s="170"/>
+      <c r="U24" s="170"/>
+      <c r="V24" s="170"/>
+      <c r="W24" s="170"/>
+      <c r="X24" s="170"/>
+      <c r="Y24" s="170"/>
+      <c r="Z24" s="170"/>
+      <c r="AA24" s="170"/>
+      <c r="AB24" s="170"/>
+      <c r="AC24" s="170"/>
+      <c r="AD24" s="170"/>
+      <c r="AE24" s="170"/>
+      <c r="AF24" s="170"/>
+      <c r="AG24" s="170"/>
+      <c r="AH24" s="170"/>
+      <c r="AI24" s="170"/>
+      <c r="AJ24" s="170"/>
+      <c r="AK24" s="170"/>
+      <c r="AL24" s="170"/>
+      <c r="AM24" s="170"/>
+      <c r="AN24" s="170"/>
       <c r="AO24" s="57"/>
       <c r="AP24" s="57"/>
       <c r="AQ24" s="57"/>
@@ -5042,7 +5129,7 @@
       <c r="J26" s="57"/>
       <c r="K26" s="57"/>
       <c r="L26" s="131" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M26" s="57"/>
       <c r="N26" s="57"/>
@@ -5078,7 +5165,7 @@
       <c r="AR26" s="57"/>
       <c r="AS26" s="57"/>
       <c r="AT26" s="79" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AU26" s="57"/>
       <c r="AV26" s="57"/>
@@ -5097,7 +5184,7 @@
       <c r="G27" s="78"/>
       <c r="H27" s="78"/>
       <c r="I27" s="147" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J27" s="122"/>
       <c r="K27" s="119"/>
@@ -5135,7 +5222,7 @@
       <c r="AQ27" s="123"/>
       <c r="AR27" s="124"/>
       <c r="AS27" s="125" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AT27" s="124"/>
       <c r="AU27" s="124"/>
@@ -6231,7 +6318,7 @@
       <c r="D48" s="57"/>
       <c r="E48" s="57"/>
       <c r="F48" s="79" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G48" s="57"/>
       <c r="H48" s="57"/>
@@ -6596,11 +6683,11 @@
     </row>
     <row r="55" spans="1:52" ht="13.8" customHeight="1">
       <c r="C55" s="133" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D55" s="57"/>
       <c r="E55" s="127" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F55" s="57"/>
       <c r="G55" s="57"/>
@@ -6647,11 +6734,11 @@
       <c r="A56" s="57"/>
       <c r="B56" s="57"/>
       <c r="C56" s="132" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D56" s="57"/>
       <c r="E56" s="81" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F56" s="57"/>
       <c r="G56" s="57"/>
@@ -6705,11 +6792,11 @@
       <c r="A57" s="57"/>
       <c r="B57" s="57"/>
       <c r="C57" s="132" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D57" s="57"/>
       <c r="E57" s="81" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F57" s="57"/>
       <c r="G57" s="57"/>
@@ -6764,11 +6851,11 @@
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
       <c r="D58" s="132" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E58" s="57"/>
       <c r="F58" s="134" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G58" s="135"/>
       <c r="H58" s="135"/>
@@ -6822,11 +6909,11 @@
       <c r="B59" s="57"/>
       <c r="C59" s="57"/>
       <c r="D59" s="132" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E59" s="57"/>
       <c r="F59" s="81" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G59" s="57"/>
       <c r="H59" s="57"/>
@@ -6880,11 +6967,11 @@
       <c r="B60" s="57"/>
       <c r="C60" s="57"/>
       <c r="D60" s="132" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E60" s="57"/>
       <c r="F60" s="81" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G60" s="57"/>
       <c r="H60" s="57"/>
@@ -7583,7 +7670,7 @@
     </row>
     <row r="73" spans="1:52">
       <c r="A73" s="156" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B73" s="157"/>
       <c r="C73" s="157"/>
@@ -7765,18 +7852,18 @@
       <c r="Q76" s="57"/>
       <c r="R76" s="57"/>
       <c r="S76" s="57"/>
-      <c r="T76" s="166" t="s">
-        <v>59</v>
+      <c r="T76" s="162" t="s">
+        <v>57</v>
       </c>
-      <c r="U76" s="166"/>
-      <c r="V76" s="166"/>
-      <c r="W76" s="166"/>
-      <c r="X76" s="166"/>
-      <c r="Y76" s="166"/>
-      <c r="Z76" s="166"/>
-      <c r="AA76" s="166"/>
-      <c r="AB76" s="166"/>
-      <c r="AC76" s="166"/>
+      <c r="U76" s="162"/>
+      <c r="V76" s="162"/>
+      <c r="W76" s="162"/>
+      <c r="X76" s="162"/>
+      <c r="Y76" s="162"/>
+      <c r="Z76" s="162"/>
+      <c r="AA76" s="162"/>
+      <c r="AB76" s="162"/>
+      <c r="AC76" s="162"/>
       <c r="AD76" s="57"/>
       <c r="AE76" s="57"/>
       <c r="AF76" s="57"/>
@@ -7821,16 +7908,16 @@
       <c r="Q77" s="57"/>
       <c r="R77" s="57"/>
       <c r="S77" s="57"/>
-      <c r="T77" s="166"/>
-      <c r="U77" s="166"/>
-      <c r="V77" s="166"/>
-      <c r="W77" s="166"/>
-      <c r="X77" s="166"/>
-      <c r="Y77" s="166"/>
-      <c r="Z77" s="166"/>
-      <c r="AA77" s="166"/>
-      <c r="AB77" s="166"/>
-      <c r="AC77" s="166"/>
+      <c r="T77" s="162"/>
+      <c r="U77" s="162"/>
+      <c r="V77" s="162"/>
+      <c r="W77" s="162"/>
+      <c r="X77" s="162"/>
+      <c r="Y77" s="162"/>
+      <c r="Z77" s="162"/>
+      <c r="AA77" s="162"/>
+      <c r="AB77" s="162"/>
+      <c r="AC77" s="162"/>
       <c r="AD77" s="57"/>
       <c r="AE77" s="57"/>
       <c r="AF77" s="57"/>
@@ -7875,16 +7962,16 @@
       <c r="Q78" s="129"/>
       <c r="R78" s="130"/>
       <c r="S78" s="130"/>
-      <c r="T78" s="166"/>
-      <c r="U78" s="166"/>
-      <c r="V78" s="166"/>
-      <c r="W78" s="166"/>
-      <c r="X78" s="166"/>
-      <c r="Y78" s="166"/>
-      <c r="Z78" s="166"/>
-      <c r="AA78" s="166"/>
-      <c r="AB78" s="166"/>
-      <c r="AC78" s="166"/>
+      <c r="T78" s="162"/>
+      <c r="U78" s="162"/>
+      <c r="V78" s="162"/>
+      <c r="W78" s="162"/>
+      <c r="X78" s="162"/>
+      <c r="Y78" s="162"/>
+      <c r="Z78" s="162"/>
+      <c r="AA78" s="162"/>
+      <c r="AB78" s="162"/>
+      <c r="AC78" s="162"/>
       <c r="AD78" s="57"/>
       <c r="AE78" s="57"/>
       <c r="AF78" s="57"/>
@@ -7979,7 +8066,7 @@
       <c r="M80" s="88"/>
       <c r="N80" s="57"/>
       <c r="O80" s="152" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="P80" s="57"/>
       <c r="Q80" s="57"/>
@@ -8089,7 +8176,7 @@
       <c r="M82" s="88"/>
       <c r="N82" s="74"/>
       <c r="O82" s="146" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P82" s="71"/>
       <c r="Q82" s="144"/>
@@ -8253,7 +8340,7 @@
       <c r="M85" s="88"/>
       <c r="N85" s="57"/>
       <c r="O85" s="152" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P85" s="57"/>
       <c r="Q85" s="57"/>
@@ -8363,7 +8450,7 @@
       <c r="M87" s="88"/>
       <c r="N87" s="80"/>
       <c r="O87" s="149" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P87" s="119"/>
       <c r="Q87" s="119"/>
@@ -8585,17 +8672,17 @@
       <c r="Q91" s="85"/>
       <c r="R91" s="83"/>
       <c r="S91" s="83"/>
-      <c r="T91" s="160" t="s">
-        <v>59</v>
+      <c r="T91" s="197" t="s">
+        <v>57</v>
       </c>
-      <c r="U91" s="161"/>
-      <c r="V91" s="161"/>
-      <c r="W91" s="161"/>
-      <c r="X91" s="161"/>
-      <c r="Y91" s="161"/>
-      <c r="Z91" s="161"/>
-      <c r="AA91" s="161"/>
-      <c r="AB91" s="162"/>
+      <c r="U91" s="198"/>
+      <c r="V91" s="198"/>
+      <c r="W91" s="198"/>
+      <c r="X91" s="198"/>
+      <c r="Y91" s="198"/>
+      <c r="Z91" s="198"/>
+      <c r="AA91" s="198"/>
+      <c r="AB91" s="199"/>
       <c r="AC91" s="83"/>
       <c r="AD91" s="83"/>
       <c r="AE91" s="83"/>
@@ -8641,15 +8728,15 @@
       <c r="Q92" s="82"/>
       <c r="R92" s="82"/>
       <c r="S92" s="82"/>
-      <c r="T92" s="163"/>
-      <c r="U92" s="164"/>
-      <c r="V92" s="164"/>
-      <c r="W92" s="164"/>
-      <c r="X92" s="164"/>
-      <c r="Y92" s="164"/>
-      <c r="Z92" s="164"/>
-      <c r="AA92" s="164"/>
-      <c r="AB92" s="165"/>
+      <c r="T92" s="200"/>
+      <c r="U92" s="201"/>
+      <c r="V92" s="201"/>
+      <c r="W92" s="201"/>
+      <c r="X92" s="201"/>
+      <c r="Y92" s="201"/>
+      <c r="Z92" s="201"/>
+      <c r="AA92" s="201"/>
+      <c r="AB92" s="202"/>
       <c r="AC92" s="82"/>
       <c r="AD92" s="82"/>
       <c r="AE92" s="82"/>
@@ -8748,7 +8835,7 @@
       <c r="R94" s="154"/>
       <c r="S94" s="154"/>
       <c r="T94" s="151" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U94" s="154"/>
       <c r="V94" s="154"/>
@@ -9071,18 +9158,18 @@
       <c r="P100" s="57"/>
       <c r="Q100" s="57"/>
       <c r="R100" s="57"/>
-      <c r="T100" s="166" t="s">
-        <v>67</v>
+      <c r="T100" s="162" t="s">
+        <v>65</v>
       </c>
-      <c r="U100" s="166"/>
-      <c r="V100" s="166"/>
-      <c r="W100" s="166"/>
-      <c r="X100" s="166"/>
-      <c r="Y100" s="166"/>
-      <c r="Z100" s="166"/>
-      <c r="AA100" s="166"/>
-      <c r="AB100" s="166"/>
-      <c r="AC100" s="166"/>
+      <c r="U100" s="162"/>
+      <c r="V100" s="162"/>
+      <c r="W100" s="162"/>
+      <c r="X100" s="162"/>
+      <c r="Y100" s="162"/>
+      <c r="Z100" s="162"/>
+      <c r="AA100" s="162"/>
+      <c r="AB100" s="162"/>
+      <c r="AC100" s="162"/>
       <c r="AD100" s="153"/>
       <c r="AE100" s="57"/>
       <c r="AF100" s="57"/>
@@ -9127,16 +9214,16 @@
       <c r="Q101" s="57"/>
       <c r="R101" s="57"/>
       <c r="S101" s="153"/>
-      <c r="T101" s="166"/>
-      <c r="U101" s="166"/>
-      <c r="V101" s="166"/>
-      <c r="W101" s="166"/>
-      <c r="X101" s="166"/>
-      <c r="Y101" s="166"/>
-      <c r="Z101" s="166"/>
-      <c r="AA101" s="166"/>
-      <c r="AB101" s="166"/>
-      <c r="AC101" s="166"/>
+      <c r="T101" s="162"/>
+      <c r="U101" s="162"/>
+      <c r="V101" s="162"/>
+      <c r="W101" s="162"/>
+      <c r="X101" s="162"/>
+      <c r="Y101" s="162"/>
+      <c r="Z101" s="162"/>
+      <c r="AA101" s="162"/>
+      <c r="AB101" s="162"/>
+      <c r="AC101" s="162"/>
       <c r="AD101" s="153"/>
       <c r="AE101" s="57"/>
       <c r="AF101" s="57"/>
@@ -9181,16 +9268,16 @@
       <c r="Q102" s="57"/>
       <c r="R102" s="57"/>
       <c r="S102" s="153"/>
-      <c r="T102" s="166"/>
-      <c r="U102" s="166"/>
-      <c r="V102" s="166"/>
-      <c r="W102" s="166"/>
-      <c r="X102" s="166"/>
-      <c r="Y102" s="166"/>
-      <c r="Z102" s="166"/>
-      <c r="AA102" s="166"/>
-      <c r="AB102" s="166"/>
-      <c r="AC102" s="166"/>
+      <c r="T102" s="162"/>
+      <c r="U102" s="162"/>
+      <c r="V102" s="162"/>
+      <c r="W102" s="162"/>
+      <c r="X102" s="162"/>
+      <c r="Y102" s="162"/>
+      <c r="Z102" s="162"/>
+      <c r="AA102" s="162"/>
+      <c r="AB102" s="162"/>
+      <c r="AC102" s="162"/>
       <c r="AD102" s="153"/>
       <c r="AE102" s="57"/>
       <c r="AF102" s="57"/>
@@ -9339,7 +9426,7 @@
       <c r="M105" s="88"/>
       <c r="N105" s="57"/>
       <c r="O105" s="152" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P105" s="57"/>
       <c r="Q105" s="57"/>
@@ -9449,7 +9536,7 @@
       <c r="M107" s="88"/>
       <c r="N107" s="57"/>
       <c r="O107" s="149" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P107" s="119"/>
       <c r="Q107" s="119"/>
@@ -9559,7 +9646,7 @@
       <c r="M109" s="88"/>
       <c r="N109" s="57"/>
       <c r="O109" s="152" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P109" s="57"/>
       <c r="Q109" s="57"/>
@@ -9669,7 +9756,7 @@
       <c r="M111" s="88"/>
       <c r="N111" s="57"/>
       <c r="O111" s="149" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P111" s="119"/>
       <c r="Q111" s="119"/>
@@ -9779,7 +9866,7 @@
       <c r="M113" s="88"/>
       <c r="N113" s="57"/>
       <c r="O113" s="152" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P113" s="57"/>
       <c r="Q113" s="57"/>
@@ -9889,7 +9976,7 @@
       <c r="M115" s="88"/>
       <c r="N115" s="57"/>
       <c r="O115" s="149" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P115" s="119"/>
       <c r="Q115" s="119"/>
@@ -9999,7 +10086,7 @@
       <c r="M117" s="88"/>
       <c r="N117" s="57"/>
       <c r="O117" s="152" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P117" s="57"/>
       <c r="Q117" s="57"/>
@@ -10109,7 +10196,7 @@
       <c r="M119" s="88"/>
       <c r="N119" s="57"/>
       <c r="O119" s="149" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P119" s="119"/>
       <c r="Q119" s="119"/>
@@ -10219,7 +10306,7 @@
       <c r="M121" s="88"/>
       <c r="N121" s="57"/>
       <c r="O121" s="152" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P121" s="57"/>
       <c r="Q121" s="57"/>
@@ -10329,7 +10416,7 @@
       <c r="M123" s="88"/>
       <c r="N123" s="57"/>
       <c r="O123" s="149" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P123" s="119"/>
       <c r="Q123" s="119"/>
@@ -10497,17 +10584,17 @@
       <c r="Q126" s="57"/>
       <c r="R126" s="57"/>
       <c r="S126" s="57"/>
-      <c r="T126" s="160" t="s">
-        <v>67</v>
+      <c r="T126" s="197" t="s">
+        <v>65</v>
       </c>
-      <c r="U126" s="167"/>
-      <c r="V126" s="167"/>
-      <c r="W126" s="167"/>
-      <c r="X126" s="167"/>
-      <c r="Y126" s="167"/>
-      <c r="Z126" s="167"/>
-      <c r="AA126" s="167"/>
-      <c r="AB126" s="168"/>
+      <c r="U126" s="203"/>
+      <c r="V126" s="203"/>
+      <c r="W126" s="203"/>
+      <c r="X126" s="203"/>
+      <c r="Y126" s="203"/>
+      <c r="Z126" s="203"/>
+      <c r="AA126" s="203"/>
+      <c r="AB126" s="204"/>
       <c r="AC126" s="57"/>
       <c r="AD126" s="57"/>
       <c r="AE126" s="57"/>
@@ -10553,15 +10640,15 @@
       <c r="Q127" s="57"/>
       <c r="R127" s="57"/>
       <c r="S127" s="57"/>
-      <c r="T127" s="169"/>
-      <c r="U127" s="170"/>
-      <c r="V127" s="170"/>
-      <c r="W127" s="170"/>
-      <c r="X127" s="170"/>
-      <c r="Y127" s="170"/>
-      <c r="Z127" s="170"/>
-      <c r="AA127" s="170"/>
-      <c r="AB127" s="171"/>
+      <c r="T127" s="205"/>
+      <c r="U127" s="206"/>
+      <c r="V127" s="206"/>
+      <c r="W127" s="206"/>
+      <c r="X127" s="206"/>
+      <c r="Y127" s="206"/>
+      <c r="Z127" s="206"/>
+      <c r="AA127" s="206"/>
+      <c r="AB127" s="207"/>
       <c r="AC127" s="57"/>
       <c r="AD127" s="57"/>
       <c r="AE127" s="57"/>
@@ -10803,9 +10890,1555 @@
       <c r="AY131" s="57"/>
       <c r="AZ131" s="57"/>
     </row>
+    <row r="133" spans="1:52">
+      <c r="A133" s="156" t="s">
+        <v>80</v>
+      </c>
+      <c r="B133" s="157"/>
+      <c r="C133" s="157"/>
+      <c r="D133" s="157"/>
+      <c r="E133" s="157"/>
+      <c r="F133" s="157"/>
+      <c r="G133" s="157"/>
+      <c r="H133" s="157"/>
+      <c r="I133" s="157"/>
+      <c r="J133" s="157"/>
+      <c r="K133" s="157"/>
+      <c r="L133" s="157"/>
+      <c r="M133" s="157"/>
+      <c r="N133" s="157"/>
+      <c r="O133" s="157"/>
+      <c r="P133" s="157"/>
+      <c r="Q133" s="157"/>
+      <c r="R133" s="157"/>
+      <c r="S133" s="157"/>
+      <c r="T133" s="157"/>
+      <c r="U133" s="157"/>
+      <c r="V133" s="157"/>
+      <c r="W133" s="157"/>
+      <c r="X133" s="157"/>
+      <c r="Y133" s="157"/>
+      <c r="Z133" s="157"/>
+      <c r="AA133" s="157"/>
+      <c r="AB133" s="157"/>
+      <c r="AC133" s="157"/>
+      <c r="AD133" s="157"/>
+      <c r="AE133" s="157"/>
+      <c r="AF133" s="157"/>
+      <c r="AG133" s="157"/>
+      <c r="AH133" s="157"/>
+      <c r="AI133" s="157"/>
+      <c r="AJ133" s="157"/>
+      <c r="AK133" s="157"/>
+      <c r="AL133" s="157"/>
+      <c r="AM133" s="157"/>
+      <c r="AN133" s="157"/>
+      <c r="AO133" s="157"/>
+      <c r="AP133" s="157"/>
+      <c r="AQ133" s="157"/>
+      <c r="AR133" s="157"/>
+      <c r="AS133" s="157"/>
+      <c r="AT133" s="157"/>
+      <c r="AU133" s="157"/>
+      <c r="AV133" s="158"/>
+    </row>
+    <row r="134" spans="1:52" ht="14.4" thickBot="1"/>
+    <row r="135" spans="1:52">
+      <c r="B135" s="93"/>
+      <c r="C135" s="94"/>
+      <c r="D135" s="94"/>
+      <c r="E135" s="94"/>
+      <c r="F135" s="94"/>
+      <c r="G135" s="94"/>
+      <c r="H135" s="94"/>
+      <c r="I135" s="94"/>
+      <c r="J135" s="94"/>
+      <c r="K135" s="94"/>
+      <c r="L135" s="94"/>
+      <c r="M135" s="94"/>
+      <c r="N135" s="94"/>
+      <c r="O135" s="94"/>
+      <c r="P135" s="94"/>
+      <c r="Q135" s="94"/>
+      <c r="R135" s="94"/>
+      <c r="S135" s="94"/>
+      <c r="T135" s="94"/>
+      <c r="U135" s="94"/>
+      <c r="V135" s="94"/>
+      <c r="W135" s="94"/>
+      <c r="X135" s="94"/>
+      <c r="Y135" s="94"/>
+      <c r="Z135" s="94"/>
+      <c r="AA135" s="94"/>
+      <c r="AB135" s="94"/>
+      <c r="AC135" s="94"/>
+      <c r="AD135" s="94"/>
+      <c r="AE135" s="94"/>
+      <c r="AF135" s="94"/>
+      <c r="AG135" s="94"/>
+      <c r="AH135" s="94"/>
+      <c r="AI135" s="94"/>
+      <c r="AJ135" s="94"/>
+      <c r="AK135" s="94"/>
+      <c r="AL135" s="94"/>
+      <c r="AM135" s="94"/>
+      <c r="AN135" s="94"/>
+      <c r="AO135" s="94"/>
+      <c r="AP135" s="94"/>
+      <c r="AQ135" s="94"/>
+      <c r="AR135" s="94"/>
+      <c r="AS135" s="94"/>
+      <c r="AT135" s="94"/>
+      <c r="AU135" s="94"/>
+      <c r="AV135" s="97"/>
+    </row>
+    <row r="136" spans="1:52" ht="24.6">
+      <c r="B136" s="98"/>
+      <c r="C136" s="99"/>
+      <c r="D136" s="99"/>
+      <c r="E136" s="116" t="s">
+        <v>35</v>
+      </c>
+      <c r="F136" s="99"/>
+      <c r="G136" s="99"/>
+      <c r="H136" s="99"/>
+      <c r="I136" s="99"/>
+      <c r="J136" s="99"/>
+      <c r="K136" s="99"/>
+      <c r="L136" s="99"/>
+      <c r="M136" s="99"/>
+      <c r="N136" s="99"/>
+      <c r="O136" s="99"/>
+      <c r="P136" s="99"/>
+      <c r="Q136" s="99"/>
+      <c r="R136" s="99"/>
+      <c r="S136" s="99"/>
+      <c r="T136" s="99"/>
+      <c r="U136" s="99"/>
+      <c r="V136" s="99"/>
+      <c r="W136" s="99"/>
+      <c r="X136" s="99"/>
+      <c r="Y136" s="99"/>
+      <c r="Z136" s="99"/>
+      <c r="AA136" s="99"/>
+      <c r="AB136" s="99"/>
+      <c r="AC136" s="99"/>
+      <c r="AD136" s="99"/>
+      <c r="AE136" s="99"/>
+      <c r="AF136" s="99"/>
+      <c r="AG136" s="99"/>
+      <c r="AH136" s="99"/>
+      <c r="AI136" s="99"/>
+      <c r="AJ136" s="99"/>
+      <c r="AK136" s="99"/>
+      <c r="AL136" s="99"/>
+      <c r="AM136" s="99"/>
+      <c r="AN136" s="99"/>
+      <c r="AO136" s="99"/>
+      <c r="AP136" s="99"/>
+      <c r="AQ136" s="99"/>
+      <c r="AR136" s="99"/>
+      <c r="AS136" s="99"/>
+      <c r="AT136" s="99"/>
+      <c r="AU136" s="99"/>
+      <c r="AV136" s="103"/>
+    </row>
+    <row r="137" spans="1:52" ht="14.4" thickBot="1">
+      <c r="B137" s="104"/>
+      <c r="C137" s="105"/>
+      <c r="D137" s="105"/>
+      <c r="E137" s="105"/>
+      <c r="F137" s="105"/>
+      <c r="G137" s="105"/>
+      <c r="H137" s="105"/>
+      <c r="I137" s="105"/>
+      <c r="J137" s="105"/>
+      <c r="K137" s="105"/>
+      <c r="L137" s="105"/>
+      <c r="M137" s="105"/>
+      <c r="N137" s="105"/>
+      <c r="O137" s="105"/>
+      <c r="P137" s="105"/>
+      <c r="Q137" s="105"/>
+      <c r="R137" s="105"/>
+      <c r="S137" s="105"/>
+      <c r="T137" s="105"/>
+      <c r="U137" s="105"/>
+      <c r="V137" s="105"/>
+      <c r="W137" s="105"/>
+      <c r="X137" s="105"/>
+      <c r="Y137" s="105"/>
+      <c r="Z137" s="105"/>
+      <c r="AA137" s="105"/>
+      <c r="AB137" s="105"/>
+      <c r="AC137" s="105"/>
+      <c r="AD137" s="105"/>
+      <c r="AE137" s="105"/>
+      <c r="AF137" s="105"/>
+      <c r="AG137" s="105"/>
+      <c r="AH137" s="105"/>
+      <c r="AI137" s="105"/>
+      <c r="AJ137" s="105"/>
+      <c r="AK137" s="105"/>
+      <c r="AL137" s="105"/>
+      <c r="AM137" s="105"/>
+      <c r="AN137" s="105"/>
+      <c r="AO137" s="105"/>
+      <c r="AP137" s="105"/>
+      <c r="AQ137" s="105"/>
+      <c r="AR137" s="105"/>
+      <c r="AS137" s="105"/>
+      <c r="AT137" s="105"/>
+      <c r="AU137" s="105"/>
+      <c r="AV137" s="271"/>
+    </row>
+    <row r="138" spans="1:52">
+      <c r="B138" s="88"/>
+      <c r="C138" s="57"/>
+      <c r="D138" s="57"/>
+      <c r="E138" s="57"/>
+      <c r="F138" s="57"/>
+      <c r="G138" s="57"/>
+      <c r="H138" s="57"/>
+      <c r="I138" s="57"/>
+      <c r="J138" s="57"/>
+      <c r="K138" s="57"/>
+      <c r="L138" s="57"/>
+      <c r="M138" s="57"/>
+      <c r="N138" s="57"/>
+      <c r="O138" s="57"/>
+      <c r="P138" s="57"/>
+      <c r="Q138" s="57"/>
+      <c r="R138" s="57"/>
+      <c r="S138" s="57"/>
+      <c r="T138" s="57"/>
+      <c r="U138" s="57"/>
+      <c r="V138" s="57"/>
+      <c r="W138" s="57"/>
+      <c r="X138" s="57"/>
+      <c r="Y138" s="57"/>
+      <c r="Z138" s="57"/>
+      <c r="AA138" s="57"/>
+      <c r="AB138" s="57"/>
+      <c r="AC138" s="57"/>
+      <c r="AD138" s="57"/>
+      <c r="AE138" s="57"/>
+      <c r="AF138" s="57"/>
+      <c r="AG138" s="57"/>
+      <c r="AH138" s="57"/>
+      <c r="AI138" s="57"/>
+      <c r="AJ138" s="57"/>
+      <c r="AK138" s="57"/>
+      <c r="AL138" s="57"/>
+      <c r="AM138" s="57"/>
+      <c r="AN138" s="57"/>
+      <c r="AO138" s="57"/>
+      <c r="AP138" s="57"/>
+      <c r="AQ138" s="57"/>
+      <c r="AR138" s="57"/>
+      <c r="AS138" s="57"/>
+      <c r="AT138" s="57"/>
+      <c r="AU138" s="57"/>
+      <c r="AV138" s="89"/>
+    </row>
+    <row r="139" spans="1:52">
+      <c r="B139" s="88"/>
+      <c r="C139" s="57"/>
+      <c r="D139" s="57"/>
+      <c r="E139" s="57"/>
+      <c r="F139" s="57"/>
+      <c r="G139" s="57"/>
+      <c r="H139" s="57"/>
+      <c r="I139" s="57"/>
+      <c r="J139" s="57"/>
+      <c r="K139" s="57"/>
+      <c r="L139" s="57"/>
+      <c r="M139" s="57"/>
+      <c r="N139" s="57"/>
+      <c r="O139" s="57"/>
+      <c r="P139" s="57"/>
+      <c r="Q139" s="57"/>
+      <c r="R139" s="57"/>
+      <c r="S139" s="57"/>
+      <c r="T139" s="57"/>
+      <c r="U139" s="57"/>
+      <c r="V139" s="57"/>
+      <c r="W139" s="57"/>
+      <c r="X139" s="57"/>
+      <c r="Y139" s="57"/>
+      <c r="Z139" s="57"/>
+      <c r="AA139" s="57"/>
+      <c r="AB139" s="57"/>
+      <c r="AC139" s="57"/>
+      <c r="AD139" s="57"/>
+      <c r="AE139" s="57"/>
+      <c r="AF139" s="57"/>
+      <c r="AG139" s="57"/>
+      <c r="AH139" s="57"/>
+      <c r="AI139" s="57"/>
+      <c r="AJ139" s="57"/>
+      <c r="AK139" s="57"/>
+      <c r="AL139" s="57"/>
+      <c r="AM139" s="57"/>
+      <c r="AN139" s="57"/>
+      <c r="AO139" s="57"/>
+      <c r="AP139" s="57"/>
+      <c r="AQ139" s="57"/>
+      <c r="AR139" s="57"/>
+      <c r="AS139" s="57"/>
+      <c r="AT139" s="57"/>
+      <c r="AU139" s="57"/>
+      <c r="AV139" s="89"/>
+    </row>
+    <row r="140" spans="1:52">
+      <c r="B140" s="88"/>
+      <c r="C140" s="57"/>
+      <c r="D140" s="57"/>
+      <c r="E140" s="57"/>
+      <c r="F140" s="57"/>
+      <c r="G140" s="57"/>
+      <c r="H140" s="57"/>
+      <c r="I140" s="57"/>
+      <c r="J140" s="57"/>
+      <c r="K140" s="57"/>
+      <c r="L140" s="57"/>
+      <c r="M140" s="57"/>
+      <c r="N140" s="57"/>
+      <c r="O140" s="57"/>
+      <c r="P140" s="57"/>
+      <c r="Q140" s="57"/>
+      <c r="R140" s="57"/>
+      <c r="S140" s="57"/>
+      <c r="T140" s="57"/>
+      <c r="U140" s="57"/>
+      <c r="V140" s="57"/>
+      <c r="W140" s="57"/>
+      <c r="X140" s="57"/>
+      <c r="Y140" s="57"/>
+      <c r="Z140" s="57"/>
+      <c r="AA140" s="57"/>
+      <c r="AB140" s="57"/>
+      <c r="AC140" s="57"/>
+      <c r="AD140" s="57"/>
+      <c r="AE140" s="57"/>
+      <c r="AF140" s="57"/>
+      <c r="AG140" s="57"/>
+      <c r="AH140" s="57"/>
+      <c r="AI140" s="57"/>
+      <c r="AJ140" s="57"/>
+      <c r="AK140" s="57"/>
+      <c r="AL140" s="57"/>
+      <c r="AM140" s="57"/>
+      <c r="AN140" s="57"/>
+      <c r="AO140" s="57"/>
+      <c r="AP140" s="57"/>
+      <c r="AQ140" s="57"/>
+      <c r="AR140" s="57"/>
+      <c r="AS140" s="57"/>
+      <c r="AT140" s="57"/>
+      <c r="AU140" s="57"/>
+      <c r="AV140" s="89"/>
+    </row>
+    <row r="141" spans="1:52">
+      <c r="B141" s="88"/>
+      <c r="C141" s="57"/>
+      <c r="D141" s="57"/>
+      <c r="E141" s="57"/>
+      <c r="F141" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="G141" s="57"/>
+      <c r="H141" s="57"/>
+      <c r="I141" s="57"/>
+      <c r="J141" s="57"/>
+      <c r="K141" s="57"/>
+      <c r="L141" s="57"/>
+      <c r="M141" s="57"/>
+      <c r="N141" s="57"/>
+      <c r="O141" s="57"/>
+      <c r="P141" s="57"/>
+      <c r="Q141" s="57"/>
+      <c r="R141" s="57"/>
+      <c r="S141" s="57"/>
+      <c r="T141" s="57"/>
+      <c r="U141" s="57"/>
+      <c r="V141" s="57"/>
+      <c r="W141" s="57"/>
+      <c r="X141" s="57"/>
+      <c r="Y141" s="57"/>
+      <c r="Z141" s="57"/>
+      <c r="AA141" s="57"/>
+      <c r="AB141" s="57"/>
+      <c r="AC141" s="57"/>
+      <c r="AD141" s="57"/>
+      <c r="AE141" s="57"/>
+      <c r="AF141" s="57"/>
+      <c r="AG141" s="57"/>
+      <c r="AH141" s="57"/>
+      <c r="AI141" s="57"/>
+      <c r="AJ141" s="57"/>
+      <c r="AK141" s="57"/>
+      <c r="AL141" s="57"/>
+      <c r="AM141" s="57"/>
+      <c r="AN141" s="57"/>
+      <c r="AO141" s="57"/>
+      <c r="AP141" s="57"/>
+      <c r="AQ141" s="57"/>
+      <c r="AR141" s="57"/>
+      <c r="AS141" s="57"/>
+      <c r="AT141" s="57"/>
+      <c r="AU141" s="57"/>
+      <c r="AV141" s="89"/>
+    </row>
+    <row r="142" spans="1:52">
+      <c r="B142" s="88"/>
+      <c r="C142" s="57"/>
+      <c r="D142" s="57"/>
+      <c r="E142" s="57"/>
+      <c r="F142" s="57"/>
+      <c r="G142" s="57"/>
+      <c r="H142" s="57"/>
+      <c r="I142" s="57"/>
+      <c r="J142" s="57"/>
+      <c r="K142" s="57"/>
+      <c r="L142" s="57"/>
+      <c r="M142" s="57"/>
+      <c r="N142" s="57"/>
+      <c r="O142" s="57"/>
+      <c r="P142" s="57"/>
+      <c r="Q142" s="57"/>
+      <c r="R142" s="57"/>
+      <c r="S142" s="57"/>
+      <c r="T142" s="57"/>
+      <c r="U142" s="57"/>
+      <c r="V142" s="57"/>
+      <c r="W142" s="57"/>
+      <c r="X142" s="57"/>
+      <c r="Y142" s="57"/>
+      <c r="Z142" s="57"/>
+      <c r="AA142" s="57"/>
+      <c r="AB142" s="57"/>
+      <c r="AC142" s="57"/>
+      <c r="AD142" s="57"/>
+      <c r="AE142" s="57"/>
+      <c r="AF142" s="57"/>
+      <c r="AG142" s="57"/>
+      <c r="AH142" s="57"/>
+      <c r="AI142" s="57"/>
+      <c r="AJ142" s="57"/>
+      <c r="AK142" s="57"/>
+      <c r="AL142" s="57"/>
+      <c r="AM142" s="57"/>
+      <c r="AN142" s="57"/>
+      <c r="AO142" s="57"/>
+      <c r="AP142" s="57"/>
+      <c r="AQ142" s="57"/>
+      <c r="AR142" s="57"/>
+      <c r="AS142" s="57"/>
+      <c r="AT142" s="57"/>
+      <c r="AU142" s="57"/>
+      <c r="AV142" s="89"/>
+    </row>
+    <row r="143" spans="1:52">
+      <c r="B143" s="88"/>
+      <c r="C143" s="57"/>
+      <c r="D143" s="57"/>
+      <c r="E143" s="57"/>
+      <c r="F143" s="149" t="s">
+        <v>82</v>
+      </c>
+      <c r="G143" s="119"/>
+      <c r="H143" s="119"/>
+      <c r="I143" s="119"/>
+      <c r="J143" s="119"/>
+      <c r="K143" s="119"/>
+      <c r="L143" s="119"/>
+      <c r="M143" s="119"/>
+      <c r="N143" s="119"/>
+      <c r="O143" s="119"/>
+      <c r="P143" s="119"/>
+      <c r="Q143" s="119"/>
+      <c r="R143" s="119"/>
+      <c r="S143" s="119"/>
+      <c r="T143" s="119"/>
+      <c r="U143" s="119"/>
+      <c r="V143" s="119"/>
+      <c r="W143" s="119"/>
+      <c r="X143" s="119"/>
+      <c r="Y143" s="119"/>
+      <c r="Z143" s="119"/>
+      <c r="AA143" s="119"/>
+      <c r="AB143" s="119"/>
+      <c r="AC143" s="119"/>
+      <c r="AD143" s="119"/>
+      <c r="AE143" s="119"/>
+      <c r="AF143" s="119"/>
+      <c r="AG143" s="119"/>
+      <c r="AH143" s="119"/>
+      <c r="AI143" s="119"/>
+      <c r="AJ143" s="119"/>
+      <c r="AK143" s="119"/>
+      <c r="AL143" s="119"/>
+      <c r="AM143" s="119"/>
+      <c r="AN143" s="119"/>
+      <c r="AO143" s="119"/>
+      <c r="AP143" s="120"/>
+      <c r="AQ143" s="57"/>
+      <c r="AR143" s="57"/>
+      <c r="AS143" s="57"/>
+      <c r="AT143" s="57"/>
+      <c r="AU143" s="57"/>
+      <c r="AV143" s="89"/>
+    </row>
+    <row r="144" spans="1:52">
+      <c r="B144" s="88"/>
+      <c r="C144" s="57"/>
+      <c r="D144" s="57"/>
+      <c r="E144" s="57"/>
+      <c r="F144" s="57"/>
+      <c r="G144" s="57"/>
+      <c r="H144" s="57"/>
+      <c r="I144" s="57"/>
+      <c r="J144" s="57"/>
+      <c r="K144" s="57"/>
+      <c r="L144" s="57"/>
+      <c r="M144" s="57"/>
+      <c r="N144" s="57"/>
+      <c r="O144" s="57"/>
+      <c r="P144" s="57"/>
+      <c r="Q144" s="57"/>
+      <c r="R144" s="57"/>
+      <c r="S144" s="57"/>
+      <c r="T144" s="57"/>
+      <c r="U144" s="57"/>
+      <c r="V144" s="57"/>
+      <c r="W144" s="57"/>
+      <c r="X144" s="57"/>
+      <c r="Y144" s="57"/>
+      <c r="Z144" s="57"/>
+      <c r="AA144" s="57"/>
+      <c r="AB144" s="57"/>
+      <c r="AC144" s="57"/>
+      <c r="AD144" s="57"/>
+      <c r="AE144" s="57"/>
+      <c r="AF144" s="57"/>
+      <c r="AG144" s="57"/>
+      <c r="AH144" s="57"/>
+      <c r="AI144" s="57"/>
+      <c r="AJ144" s="57"/>
+      <c r="AK144" s="57"/>
+      <c r="AL144" s="57"/>
+      <c r="AM144" s="57"/>
+      <c r="AN144" s="57"/>
+      <c r="AO144" s="57"/>
+      <c r="AP144" s="57"/>
+      <c r="AQ144" s="57"/>
+      <c r="AR144" s="57"/>
+      <c r="AS144" s="57"/>
+      <c r="AT144" s="57"/>
+      <c r="AU144" s="57"/>
+      <c r="AV144" s="89"/>
+    </row>
+    <row r="145" spans="2:48">
+      <c r="B145" s="88"/>
+      <c r="C145" s="57"/>
+      <c r="D145" s="57"/>
+      <c r="E145" s="57"/>
+      <c r="F145" s="57"/>
+      <c r="G145" s="57"/>
+      <c r="H145" s="57"/>
+      <c r="I145" s="57"/>
+      <c r="J145" s="57"/>
+      <c r="K145" s="57"/>
+      <c r="L145" s="57"/>
+      <c r="M145" s="57"/>
+      <c r="N145" s="57"/>
+      <c r="O145" s="57"/>
+      <c r="P145" s="57"/>
+      <c r="Q145" s="57"/>
+      <c r="R145" s="57"/>
+      <c r="S145" s="57"/>
+      <c r="T145" s="57"/>
+      <c r="U145" s="57"/>
+      <c r="V145" s="57"/>
+      <c r="W145" s="57"/>
+      <c r="X145" s="57"/>
+      <c r="Y145" s="57"/>
+      <c r="Z145" s="57"/>
+      <c r="AA145" s="57"/>
+      <c r="AB145" s="57"/>
+      <c r="AC145" s="57"/>
+      <c r="AD145" s="57"/>
+      <c r="AE145" s="57"/>
+      <c r="AF145" s="57"/>
+      <c r="AG145" s="57"/>
+      <c r="AH145" s="57"/>
+      <c r="AI145" s="57"/>
+      <c r="AJ145" s="57"/>
+      <c r="AK145" s="57"/>
+      <c r="AL145" s="57"/>
+      <c r="AM145" s="57"/>
+      <c r="AN145" s="57"/>
+      <c r="AO145" s="57"/>
+      <c r="AP145" s="57"/>
+      <c r="AQ145" s="57"/>
+      <c r="AR145" s="57"/>
+      <c r="AS145" s="57"/>
+      <c r="AT145" s="57"/>
+      <c r="AU145" s="57"/>
+      <c r="AV145" s="89"/>
+    </row>
+    <row r="146" spans="2:48">
+      <c r="B146" s="88"/>
+      <c r="C146" s="57"/>
+      <c r="D146" s="57"/>
+      <c r="E146" s="57"/>
+      <c r="F146" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="G146" s="57"/>
+      <c r="H146" s="57"/>
+      <c r="I146" s="57"/>
+      <c r="J146" s="57"/>
+      <c r="K146" s="57"/>
+      <c r="L146" s="57"/>
+      <c r="M146" s="57"/>
+      <c r="N146" s="57"/>
+      <c r="O146" s="57"/>
+      <c r="P146" s="57"/>
+      <c r="Q146" s="57"/>
+      <c r="R146" s="57"/>
+      <c r="S146" s="57"/>
+      <c r="T146" s="57"/>
+      <c r="U146" s="57"/>
+      <c r="V146" s="57"/>
+      <c r="W146" s="57"/>
+      <c r="X146" s="57"/>
+      <c r="Y146" s="57"/>
+      <c r="Z146" s="57"/>
+      <c r="AA146" s="57"/>
+      <c r="AB146" s="57"/>
+      <c r="AC146" s="57"/>
+      <c r="AD146" s="57"/>
+      <c r="AE146" s="57"/>
+      <c r="AF146" s="57"/>
+      <c r="AG146" s="57"/>
+      <c r="AH146" s="57"/>
+      <c r="AI146" s="57"/>
+      <c r="AJ146" s="57"/>
+      <c r="AK146" s="57"/>
+      <c r="AL146" s="57"/>
+      <c r="AM146" s="57"/>
+      <c r="AN146" s="57"/>
+      <c r="AO146" s="57"/>
+      <c r="AP146" s="57"/>
+      <c r="AQ146" s="57"/>
+      <c r="AR146" s="57"/>
+      <c r="AS146" s="57"/>
+      <c r="AT146" s="57"/>
+      <c r="AU146" s="57"/>
+      <c r="AV146" s="89"/>
+    </row>
+    <row r="147" spans="2:48">
+      <c r="B147" s="88"/>
+      <c r="C147" s="57"/>
+      <c r="D147" s="57"/>
+      <c r="E147" s="57"/>
+      <c r="F147" s="57"/>
+      <c r="G147" s="57"/>
+      <c r="H147" s="57"/>
+      <c r="I147" s="57"/>
+      <c r="J147" s="57"/>
+      <c r="K147" s="57"/>
+      <c r="L147" s="57"/>
+      <c r="M147" s="57"/>
+      <c r="N147" s="57"/>
+      <c r="O147" s="57"/>
+      <c r="P147" s="57"/>
+      <c r="Q147" s="57"/>
+      <c r="R147" s="57"/>
+      <c r="S147" s="57"/>
+      <c r="T147" s="57"/>
+      <c r="U147" s="57"/>
+      <c r="V147" s="57"/>
+      <c r="W147" s="57"/>
+      <c r="X147" s="57"/>
+      <c r="Y147" s="57"/>
+      <c r="Z147" s="57"/>
+      <c r="AA147" s="57"/>
+      <c r="AB147" s="57"/>
+      <c r="AC147" s="57"/>
+      <c r="AD147" s="57"/>
+      <c r="AE147" s="57"/>
+      <c r="AF147" s="57"/>
+      <c r="AG147" s="57"/>
+      <c r="AH147" s="57"/>
+      <c r="AI147" s="57"/>
+      <c r="AJ147" s="57"/>
+      <c r="AK147" s="57"/>
+      <c r="AL147" s="57"/>
+      <c r="AM147" s="57"/>
+      <c r="AN147" s="57"/>
+      <c r="AO147" s="57"/>
+      <c r="AP147" s="57"/>
+      <c r="AQ147" s="57"/>
+      <c r="AR147" s="57"/>
+      <c r="AS147" s="57"/>
+      <c r="AT147" s="57"/>
+      <c r="AU147" s="57"/>
+      <c r="AV147" s="89"/>
+    </row>
+    <row r="148" spans="2:48">
+      <c r="B148" s="88"/>
+      <c r="C148" s="57"/>
+      <c r="D148" s="57"/>
+      <c r="E148" s="57"/>
+      <c r="F148" s="149" t="s">
+        <v>84</v>
+      </c>
+      <c r="G148" s="119"/>
+      <c r="H148" s="119"/>
+      <c r="I148" s="119"/>
+      <c r="J148" s="119"/>
+      <c r="K148" s="119"/>
+      <c r="L148" s="119"/>
+      <c r="M148" s="119"/>
+      <c r="N148" s="119"/>
+      <c r="O148" s="119"/>
+      <c r="P148" s="119"/>
+      <c r="Q148" s="119"/>
+      <c r="R148" s="119"/>
+      <c r="S148" s="119"/>
+      <c r="T148" s="119"/>
+      <c r="U148" s="119"/>
+      <c r="V148" s="119"/>
+      <c r="W148" s="119"/>
+      <c r="X148" s="119"/>
+      <c r="Y148" s="119"/>
+      <c r="Z148" s="119"/>
+      <c r="AA148" s="119"/>
+      <c r="AB148" s="119"/>
+      <c r="AC148" s="119"/>
+      <c r="AD148" s="119"/>
+      <c r="AE148" s="119"/>
+      <c r="AF148" s="119"/>
+      <c r="AG148" s="119"/>
+      <c r="AH148" s="119"/>
+      <c r="AI148" s="119"/>
+      <c r="AJ148" s="119"/>
+      <c r="AK148" s="119"/>
+      <c r="AL148" s="119"/>
+      <c r="AM148" s="119"/>
+      <c r="AN148" s="119"/>
+      <c r="AO148" s="119"/>
+      <c r="AP148" s="120"/>
+      <c r="AQ148" s="57"/>
+      <c r="AR148" s="57"/>
+      <c r="AS148" s="57"/>
+      <c r="AT148" s="57"/>
+      <c r="AU148" s="57"/>
+      <c r="AV148" s="89"/>
+    </row>
+    <row r="149" spans="2:48">
+      <c r="B149" s="88"/>
+      <c r="C149" s="57"/>
+      <c r="D149" s="57"/>
+      <c r="E149" s="57"/>
+      <c r="F149" s="57"/>
+      <c r="G149" s="57"/>
+      <c r="H149" s="57"/>
+      <c r="I149" s="57"/>
+      <c r="J149" s="57"/>
+      <c r="K149" s="57"/>
+      <c r="L149" s="57"/>
+      <c r="M149" s="57"/>
+      <c r="N149" s="57"/>
+      <c r="O149" s="57"/>
+      <c r="P149" s="57"/>
+      <c r="Q149" s="57"/>
+      <c r="R149" s="57"/>
+      <c r="S149" s="57"/>
+      <c r="T149" s="57"/>
+      <c r="U149" s="57"/>
+      <c r="V149" s="57"/>
+      <c r="W149" s="57"/>
+      <c r="X149" s="57"/>
+      <c r="Y149" s="57"/>
+      <c r="Z149" s="57"/>
+      <c r="AA149" s="57"/>
+      <c r="AB149" s="57"/>
+      <c r="AC149" s="57"/>
+      <c r="AD149" s="57"/>
+      <c r="AE149" s="57"/>
+      <c r="AF149" s="57"/>
+      <c r="AG149" s="57"/>
+      <c r="AH149" s="57"/>
+      <c r="AI149" s="57"/>
+      <c r="AJ149" s="57"/>
+      <c r="AK149" s="57"/>
+      <c r="AL149" s="57"/>
+      <c r="AM149" s="57"/>
+      <c r="AN149" s="57"/>
+      <c r="AO149" s="57"/>
+      <c r="AP149" s="57"/>
+      <c r="AQ149" s="57"/>
+      <c r="AR149" s="57"/>
+      <c r="AS149" s="57"/>
+      <c r="AT149" s="57"/>
+      <c r="AU149" s="57"/>
+      <c r="AV149" s="89"/>
+    </row>
+    <row r="150" spans="2:48">
+      <c r="B150" s="88"/>
+      <c r="C150" s="57"/>
+      <c r="D150" s="57"/>
+      <c r="E150" s="57"/>
+      <c r="F150" s="57"/>
+      <c r="G150" s="57"/>
+      <c r="H150" s="57"/>
+      <c r="I150" s="57"/>
+      <c r="J150" s="57"/>
+      <c r="K150" s="57"/>
+      <c r="L150" s="57"/>
+      <c r="M150" s="57"/>
+      <c r="N150" s="57"/>
+      <c r="O150" s="57"/>
+      <c r="P150" s="57"/>
+      <c r="Q150" s="57"/>
+      <c r="R150" s="57"/>
+      <c r="S150" s="57"/>
+      <c r="T150" s="57"/>
+      <c r="U150" s="57"/>
+      <c r="V150" s="57"/>
+      <c r="W150" s="57"/>
+      <c r="X150" s="57"/>
+      <c r="Y150" s="57"/>
+      <c r="Z150" s="57"/>
+      <c r="AA150" s="57"/>
+      <c r="AB150" s="57"/>
+      <c r="AC150" s="57"/>
+      <c r="AD150" s="57"/>
+      <c r="AE150" s="57"/>
+      <c r="AF150" s="57"/>
+      <c r="AG150" s="57"/>
+      <c r="AH150" s="57"/>
+      <c r="AI150" s="57"/>
+      <c r="AJ150" s="57"/>
+      <c r="AK150" s="57"/>
+      <c r="AL150" s="57"/>
+      <c r="AM150" s="57"/>
+      <c r="AN150" s="57"/>
+      <c r="AO150" s="57"/>
+      <c r="AP150" s="57"/>
+      <c r="AQ150" s="57"/>
+      <c r="AR150" s="57"/>
+      <c r="AS150" s="57"/>
+      <c r="AT150" s="57"/>
+      <c r="AU150" s="57"/>
+      <c r="AV150" s="89"/>
+    </row>
+    <row r="151" spans="2:48">
+      <c r="B151" s="88"/>
+      <c r="C151" s="57"/>
+      <c r="D151" s="57"/>
+      <c r="E151" s="57"/>
+      <c r="F151" s="272" t="s">
+        <v>85</v>
+      </c>
+      <c r="G151" s="57"/>
+      <c r="H151" s="57"/>
+      <c r="I151" s="57"/>
+      <c r="J151" s="57"/>
+      <c r="K151" s="57"/>
+      <c r="L151" s="57"/>
+      <c r="M151" s="57"/>
+      <c r="N151" s="57"/>
+      <c r="O151" s="57"/>
+      <c r="P151" s="57"/>
+      <c r="Q151" s="57"/>
+      <c r="R151" s="57"/>
+      <c r="S151" s="57"/>
+      <c r="T151" s="57"/>
+      <c r="U151" s="57"/>
+      <c r="V151" s="57"/>
+      <c r="W151" s="57"/>
+      <c r="X151" s="57"/>
+      <c r="Y151" s="57"/>
+      <c r="Z151" s="57"/>
+      <c r="AA151" s="57"/>
+      <c r="AB151" s="57"/>
+      <c r="AC151" s="57"/>
+      <c r="AD151" s="57"/>
+      <c r="AE151" s="57"/>
+      <c r="AF151" s="57"/>
+      <c r="AG151" s="57"/>
+      <c r="AH151" s="57"/>
+      <c r="AI151" s="57"/>
+      <c r="AJ151" s="57"/>
+      <c r="AK151" s="57"/>
+      <c r="AL151" s="57"/>
+      <c r="AM151" s="57"/>
+      <c r="AN151" s="57"/>
+      <c r="AO151" s="57"/>
+      <c r="AP151" s="57"/>
+      <c r="AQ151" s="57"/>
+      <c r="AR151" s="57"/>
+      <c r="AS151" s="57"/>
+      <c r="AT151" s="57"/>
+      <c r="AU151" s="57"/>
+      <c r="AV151" s="89"/>
+    </row>
+    <row r="152" spans="2:48">
+      <c r="B152" s="88"/>
+      <c r="C152" s="57"/>
+      <c r="D152" s="57"/>
+      <c r="E152" s="57"/>
+      <c r="F152" s="57"/>
+      <c r="G152" s="57"/>
+      <c r="H152" s="57"/>
+      <c r="I152" s="57"/>
+      <c r="J152" s="57"/>
+      <c r="K152" s="57"/>
+      <c r="L152" s="57"/>
+      <c r="M152" s="57"/>
+      <c r="N152" s="57"/>
+      <c r="O152" s="57"/>
+      <c r="P152" s="57"/>
+      <c r="Q152" s="57"/>
+      <c r="R152" s="57"/>
+      <c r="S152" s="57"/>
+      <c r="T152" s="57"/>
+      <c r="U152" s="57"/>
+      <c r="V152" s="57"/>
+      <c r="W152" s="57"/>
+      <c r="X152" s="57"/>
+      <c r="Y152" s="57"/>
+      <c r="Z152" s="57"/>
+      <c r="AA152" s="57"/>
+      <c r="AB152" s="57"/>
+      <c r="AC152" s="57"/>
+      <c r="AD152" s="57"/>
+      <c r="AE152" s="57"/>
+      <c r="AF152" s="57"/>
+      <c r="AG152" s="57"/>
+      <c r="AH152" s="57"/>
+      <c r="AI152" s="57"/>
+      <c r="AJ152" s="57"/>
+      <c r="AK152" s="57"/>
+      <c r="AL152" s="57"/>
+      <c r="AM152" s="57"/>
+      <c r="AN152" s="57"/>
+      <c r="AO152" s="57"/>
+      <c r="AP152" s="57"/>
+      <c r="AQ152" s="57"/>
+      <c r="AR152" s="57"/>
+      <c r="AS152" s="57"/>
+      <c r="AT152" s="57"/>
+      <c r="AU152" s="57"/>
+      <c r="AV152" s="89"/>
+    </row>
+    <row r="153" spans="2:48">
+      <c r="B153" s="88"/>
+      <c r="C153" s="57"/>
+      <c r="D153" s="57"/>
+      <c r="E153" s="57"/>
+      <c r="F153" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="G153" s="119"/>
+      <c r="H153" s="119"/>
+      <c r="I153" s="119"/>
+      <c r="J153" s="119"/>
+      <c r="K153" s="119"/>
+      <c r="L153" s="119"/>
+      <c r="M153" s="119"/>
+      <c r="N153" s="119"/>
+      <c r="O153" s="119"/>
+      <c r="P153" s="119"/>
+      <c r="Q153" s="119"/>
+      <c r="R153" s="119"/>
+      <c r="S153" s="119"/>
+      <c r="T153" s="119"/>
+      <c r="U153" s="119"/>
+      <c r="V153" s="119"/>
+      <c r="W153" s="119"/>
+      <c r="X153" s="119"/>
+      <c r="Y153" s="119"/>
+      <c r="Z153" s="119"/>
+      <c r="AA153" s="119"/>
+      <c r="AB153" s="119"/>
+      <c r="AC153" s="119"/>
+      <c r="AD153" s="119"/>
+      <c r="AE153" s="119"/>
+      <c r="AF153" s="119"/>
+      <c r="AG153" s="119"/>
+      <c r="AH153" s="119"/>
+      <c r="AI153" s="119"/>
+      <c r="AJ153" s="119"/>
+      <c r="AK153" s="119"/>
+      <c r="AL153" s="119"/>
+      <c r="AM153" s="119"/>
+      <c r="AN153" s="119"/>
+      <c r="AO153" s="119"/>
+      <c r="AP153" s="120"/>
+      <c r="AQ153" s="57"/>
+      <c r="AR153" s="57"/>
+      <c r="AS153" s="57"/>
+      <c r="AT153" s="57"/>
+      <c r="AU153" s="57"/>
+      <c r="AV153" s="89"/>
+    </row>
+    <row r="154" spans="2:48">
+      <c r="B154" s="88"/>
+      <c r="C154" s="57"/>
+      <c r="D154" s="57"/>
+      <c r="E154" s="57"/>
+      <c r="F154" s="57"/>
+      <c r="G154" s="57"/>
+      <c r="H154" s="57"/>
+      <c r="I154" s="57"/>
+      <c r="J154" s="57"/>
+      <c r="K154" s="57"/>
+      <c r="L154" s="57"/>
+      <c r="M154" s="57"/>
+      <c r="N154" s="57"/>
+      <c r="O154" s="57"/>
+      <c r="P154" s="57"/>
+      <c r="Q154" s="57"/>
+      <c r="R154" s="57"/>
+      <c r="S154" s="57"/>
+      <c r="T154" s="57"/>
+      <c r="U154" s="57"/>
+      <c r="V154" s="57"/>
+      <c r="W154" s="57"/>
+      <c r="X154" s="57"/>
+      <c r="Y154" s="57"/>
+      <c r="Z154" s="57"/>
+      <c r="AA154" s="57"/>
+      <c r="AB154" s="57"/>
+      <c r="AC154" s="57"/>
+      <c r="AD154" s="57"/>
+      <c r="AE154" s="57"/>
+      <c r="AF154" s="57"/>
+      <c r="AG154" s="57"/>
+      <c r="AH154" s="57"/>
+      <c r="AI154" s="57"/>
+      <c r="AJ154" s="57"/>
+      <c r="AK154" s="57"/>
+      <c r="AL154" s="57"/>
+      <c r="AM154" s="57"/>
+      <c r="AN154" s="57"/>
+      <c r="AO154" s="57"/>
+      <c r="AP154" s="57"/>
+      <c r="AQ154" s="57"/>
+      <c r="AR154" s="57"/>
+      <c r="AS154" s="57"/>
+      <c r="AT154" s="57"/>
+      <c r="AU154" s="57"/>
+      <c r="AV154" s="89"/>
+    </row>
+    <row r="155" spans="2:48">
+      <c r="B155" s="88"/>
+      <c r="C155" s="57"/>
+      <c r="D155" s="57"/>
+      <c r="E155" s="57"/>
+      <c r="F155" s="57"/>
+      <c r="G155" s="57"/>
+      <c r="H155" s="57"/>
+      <c r="I155" s="57"/>
+      <c r="J155" s="57"/>
+      <c r="K155" s="57"/>
+      <c r="L155" s="57"/>
+      <c r="M155" s="57"/>
+      <c r="N155" s="57"/>
+      <c r="O155" s="57"/>
+      <c r="P155" s="57"/>
+      <c r="Q155" s="57"/>
+      <c r="R155" s="57"/>
+      <c r="S155" s="57"/>
+      <c r="T155" s="57"/>
+      <c r="U155" s="57"/>
+      <c r="V155" s="57"/>
+      <c r="W155" s="57"/>
+      <c r="X155" s="57"/>
+      <c r="Y155" s="57"/>
+      <c r="Z155" s="57"/>
+      <c r="AA155" s="57"/>
+      <c r="AB155" s="57"/>
+      <c r="AC155" s="57"/>
+      <c r="AD155" s="57"/>
+      <c r="AE155" s="57"/>
+      <c r="AF155" s="57"/>
+      <c r="AG155" s="57"/>
+      <c r="AH155" s="57"/>
+      <c r="AI155" s="57"/>
+      <c r="AJ155" s="57"/>
+      <c r="AK155" s="57"/>
+      <c r="AL155" s="57"/>
+      <c r="AM155" s="57"/>
+      <c r="AN155" s="57"/>
+      <c r="AO155" s="57"/>
+      <c r="AP155" s="57"/>
+      <c r="AQ155" s="57"/>
+      <c r="AR155" s="57"/>
+      <c r="AS155" s="57"/>
+      <c r="AT155" s="57"/>
+      <c r="AU155" s="57"/>
+      <c r="AV155" s="89"/>
+    </row>
+    <row r="156" spans="2:48">
+      <c r="B156" s="88"/>
+      <c r="C156" s="57"/>
+      <c r="D156" s="57"/>
+      <c r="E156" s="57"/>
+      <c r="F156" s="57"/>
+      <c r="G156" s="57"/>
+      <c r="H156" s="57"/>
+      <c r="I156" s="57"/>
+      <c r="J156" s="57"/>
+      <c r="K156" s="57"/>
+      <c r="L156" s="57"/>
+      <c r="M156" s="57"/>
+      <c r="N156" s="57"/>
+      <c r="O156" s="57"/>
+      <c r="P156" s="57"/>
+      <c r="Q156" s="57"/>
+      <c r="R156" s="57"/>
+      <c r="S156" s="57"/>
+      <c r="T156" s="57"/>
+      <c r="U156" s="57"/>
+      <c r="V156" s="57"/>
+      <c r="W156" s="57"/>
+      <c r="X156" s="57"/>
+      <c r="Y156" s="57"/>
+      <c r="Z156" s="57"/>
+      <c r="AA156" s="57"/>
+      <c r="AB156" s="57"/>
+      <c r="AC156" s="57"/>
+      <c r="AD156" s="57"/>
+      <c r="AE156" s="57"/>
+      <c r="AF156" s="57"/>
+      <c r="AG156" s="57"/>
+      <c r="AH156" s="57"/>
+      <c r="AI156" s="57"/>
+      <c r="AJ156" s="57"/>
+      <c r="AK156" s="57"/>
+      <c r="AL156" s="57"/>
+      <c r="AM156" s="57"/>
+      <c r="AN156" s="57"/>
+      <c r="AO156" s="57"/>
+      <c r="AP156" s="57"/>
+      <c r="AQ156" s="57"/>
+      <c r="AR156" s="57"/>
+      <c r="AS156" s="57"/>
+      <c r="AT156" s="57"/>
+      <c r="AU156" s="57"/>
+      <c r="AV156" s="89"/>
+    </row>
+    <row r="157" spans="2:48">
+      <c r="B157" s="88"/>
+      <c r="C157" s="57"/>
+      <c r="D157" s="57"/>
+      <c r="E157" s="57"/>
+      <c r="F157" s="57"/>
+      <c r="G157" s="57"/>
+      <c r="H157" s="57"/>
+      <c r="I157" s="57"/>
+      <c r="J157" s="57"/>
+      <c r="K157" s="57"/>
+      <c r="L157" s="57"/>
+      <c r="M157" s="57"/>
+      <c r="N157" s="57"/>
+      <c r="O157" s="57"/>
+      <c r="P157" s="57"/>
+      <c r="Q157" s="57"/>
+      <c r="R157" s="57"/>
+      <c r="S157" s="57"/>
+      <c r="T157" s="57"/>
+      <c r="U157" s="57"/>
+      <c r="V157" s="57"/>
+      <c r="W157" s="57"/>
+      <c r="X157" s="57"/>
+      <c r="Y157" s="57"/>
+      <c r="Z157" s="57"/>
+      <c r="AA157" s="57"/>
+      <c r="AB157" s="57"/>
+      <c r="AC157" s="57"/>
+      <c r="AD157" s="57"/>
+      <c r="AE157" s="57"/>
+      <c r="AF157" s="57"/>
+      <c r="AG157" s="57"/>
+      <c r="AH157" s="57"/>
+      <c r="AI157" s="57"/>
+      <c r="AJ157" s="57"/>
+      <c r="AK157" s="57"/>
+      <c r="AL157" s="57"/>
+      <c r="AM157" s="57"/>
+      <c r="AN157" s="57"/>
+      <c r="AO157" s="57"/>
+      <c r="AP157" s="57"/>
+      <c r="AQ157" s="57"/>
+      <c r="AR157" s="57"/>
+      <c r="AS157" s="57"/>
+      <c r="AT157" s="57"/>
+      <c r="AU157" s="57"/>
+      <c r="AV157" s="89"/>
+    </row>
+    <row r="158" spans="2:48" ht="14.4" thickBot="1">
+      <c r="B158" s="88"/>
+      <c r="C158" s="57"/>
+      <c r="D158" s="57"/>
+      <c r="E158" s="57"/>
+      <c r="F158" s="57"/>
+      <c r="G158" s="57"/>
+      <c r="H158" s="57"/>
+      <c r="I158" s="57"/>
+      <c r="J158" s="57"/>
+      <c r="K158" s="57"/>
+      <c r="L158" s="57"/>
+      <c r="M158" s="57"/>
+      <c r="N158" s="57"/>
+      <c r="O158" s="57"/>
+      <c r="P158" s="57"/>
+      <c r="Q158" s="57"/>
+      <c r="R158" s="57"/>
+      <c r="S158" s="57"/>
+      <c r="T158" s="57"/>
+      <c r="U158" s="57"/>
+      <c r="V158" s="57"/>
+      <c r="W158" s="57"/>
+      <c r="X158" s="273" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y158" s="274"/>
+      <c r="Z158" s="275"/>
+      <c r="AA158" s="57"/>
+      <c r="AB158" s="57"/>
+      <c r="AC158" s="57"/>
+      <c r="AD158" s="57"/>
+      <c r="AE158" s="57"/>
+      <c r="AF158" s="57"/>
+      <c r="AG158" s="57"/>
+      <c r="AH158" s="57"/>
+      <c r="AI158" s="57"/>
+      <c r="AJ158" s="57"/>
+      <c r="AK158" s="57"/>
+      <c r="AL158" s="57"/>
+      <c r="AM158" s="57"/>
+      <c r="AN158" s="57"/>
+      <c r="AO158" s="57"/>
+      <c r="AP158" s="57"/>
+      <c r="AQ158" s="57"/>
+      <c r="AR158" s="57"/>
+      <c r="AS158" s="57"/>
+      <c r="AT158" s="57"/>
+      <c r="AU158" s="57"/>
+      <c r="AV158" s="89"/>
+    </row>
+    <row r="159" spans="2:48" ht="14.4" thickTop="1">
+      <c r="B159" s="88"/>
+      <c r="C159" s="57"/>
+      <c r="D159" s="57"/>
+      <c r="E159" s="57"/>
+      <c r="F159" s="57"/>
+      <c r="G159" s="57"/>
+      <c r="H159" s="57"/>
+      <c r="I159" s="57"/>
+      <c r="J159" s="57"/>
+      <c r="K159" s="57"/>
+      <c r="L159" s="57"/>
+      <c r="M159" s="57"/>
+      <c r="N159" s="57"/>
+      <c r="O159" s="57"/>
+      <c r="P159" s="57"/>
+      <c r="Q159" s="57"/>
+      <c r="R159" s="57"/>
+      <c r="S159" s="57"/>
+      <c r="T159" s="57"/>
+      <c r="U159" s="57"/>
+      <c r="V159" s="57"/>
+      <c r="W159" s="57"/>
+      <c r="X159" s="57"/>
+      <c r="Y159" s="57"/>
+      <c r="Z159" s="57"/>
+      <c r="AA159" s="57"/>
+      <c r="AB159" s="57"/>
+      <c r="AC159" s="57"/>
+      <c r="AD159" s="57"/>
+      <c r="AE159" s="57"/>
+      <c r="AF159" s="57"/>
+      <c r="AG159" s="57"/>
+      <c r="AH159" s="57"/>
+      <c r="AI159" s="57"/>
+      <c r="AJ159" s="57"/>
+      <c r="AK159" s="57"/>
+      <c r="AL159" s="57"/>
+      <c r="AM159" s="57"/>
+      <c r="AN159" s="57"/>
+      <c r="AO159" s="57"/>
+      <c r="AP159" s="57"/>
+      <c r="AQ159" s="57"/>
+      <c r="AR159" s="57"/>
+      <c r="AS159" s="57"/>
+      <c r="AT159" s="57"/>
+      <c r="AU159" s="57"/>
+      <c r="AV159" s="89"/>
+    </row>
+    <row r="160" spans="2:48">
+      <c r="B160" s="88"/>
+      <c r="C160" s="57"/>
+      <c r="D160" s="57"/>
+      <c r="E160" s="57"/>
+      <c r="F160" s="57"/>
+      <c r="G160" s="57"/>
+      <c r="H160" s="57"/>
+      <c r="I160" s="57"/>
+      <c r="J160" s="57"/>
+      <c r="K160" s="57"/>
+      <c r="L160" s="57"/>
+      <c r="M160" s="57"/>
+      <c r="N160" s="57"/>
+      <c r="O160" s="57"/>
+      <c r="P160" s="57"/>
+      <c r="Q160" s="57"/>
+      <c r="R160" s="57"/>
+      <c r="S160" s="57"/>
+      <c r="T160" s="57"/>
+      <c r="U160" s="57"/>
+      <c r="V160" s="57"/>
+      <c r="W160" s="57"/>
+      <c r="X160" s="57"/>
+      <c r="Y160" s="57"/>
+      <c r="Z160" s="57"/>
+      <c r="AA160" s="57"/>
+      <c r="AB160" s="57"/>
+      <c r="AC160" s="57"/>
+      <c r="AD160" s="57"/>
+      <c r="AE160" s="57"/>
+      <c r="AF160" s="57"/>
+      <c r="AG160" s="57"/>
+      <c r="AH160" s="57"/>
+      <c r="AI160" s="57"/>
+      <c r="AJ160" s="57"/>
+      <c r="AK160" s="57"/>
+      <c r="AL160" s="57"/>
+      <c r="AM160" s="57"/>
+      <c r="AN160" s="57"/>
+      <c r="AO160" s="57"/>
+      <c r="AP160" s="57"/>
+      <c r="AQ160" s="57"/>
+      <c r="AR160" s="57"/>
+      <c r="AS160" s="57"/>
+      <c r="AT160" s="57"/>
+      <c r="AU160" s="57"/>
+      <c r="AV160" s="89"/>
+    </row>
+    <row r="161" spans="2:48">
+      <c r="B161" s="88"/>
+      <c r="C161" s="57"/>
+      <c r="D161" s="57"/>
+      <c r="E161" s="57"/>
+      <c r="F161" s="57"/>
+      <c r="G161" s="57"/>
+      <c r="H161" s="57"/>
+      <c r="I161" s="57"/>
+      <c r="J161" s="57"/>
+      <c r="K161" s="57"/>
+      <c r="L161" s="57"/>
+      <c r="M161" s="57"/>
+      <c r="N161" s="57"/>
+      <c r="O161" s="57"/>
+      <c r="P161" s="57"/>
+      <c r="Q161" s="57"/>
+      <c r="R161" s="57"/>
+      <c r="S161" s="57"/>
+      <c r="T161" s="57"/>
+      <c r="U161" s="57"/>
+      <c r="V161" s="57"/>
+      <c r="W161" s="57"/>
+      <c r="X161" s="57"/>
+      <c r="Y161" s="57"/>
+      <c r="Z161" s="57"/>
+      <c r="AA161" s="57"/>
+      <c r="AB161" s="57"/>
+      <c r="AC161" s="57"/>
+      <c r="AD161" s="57"/>
+      <c r="AE161" s="57"/>
+      <c r="AF161" s="57"/>
+      <c r="AG161" s="57"/>
+      <c r="AH161" s="57"/>
+      <c r="AI161" s="57"/>
+      <c r="AJ161" s="57"/>
+      <c r="AK161" s="57"/>
+      <c r="AL161" s="57"/>
+      <c r="AM161" s="57"/>
+      <c r="AN161" s="57"/>
+      <c r="AO161" s="57"/>
+      <c r="AP161" s="57"/>
+      <c r="AQ161" s="57"/>
+      <c r="AR161" s="57"/>
+      <c r="AS161" s="57"/>
+      <c r="AT161" s="57"/>
+      <c r="AU161" s="57"/>
+      <c r="AV161" s="89"/>
+    </row>
+    <row r="162" spans="2:48">
+      <c r="B162" s="88"/>
+      <c r="C162" s="57"/>
+      <c r="D162" s="57"/>
+      <c r="E162" s="57"/>
+      <c r="F162" s="57"/>
+      <c r="G162" s="57"/>
+      <c r="H162" s="57"/>
+      <c r="I162" s="57"/>
+      <c r="J162" s="57"/>
+      <c r="K162" s="57"/>
+      <c r="L162" s="57"/>
+      <c r="M162" s="57"/>
+      <c r="N162" s="57"/>
+      <c r="O162" s="57"/>
+      <c r="P162" s="57"/>
+      <c r="Q162" s="57"/>
+      <c r="R162" s="57"/>
+      <c r="S162" s="57"/>
+      <c r="T162" s="57"/>
+      <c r="U162" s="57"/>
+      <c r="V162" s="57"/>
+      <c r="W162" s="57"/>
+      <c r="X162" s="57"/>
+      <c r="Y162" s="57"/>
+      <c r="Z162" s="57"/>
+      <c r="AA162" s="57"/>
+      <c r="AB162" s="57"/>
+      <c r="AC162" s="57"/>
+      <c r="AD162" s="57"/>
+      <c r="AE162" s="57"/>
+      <c r="AF162" s="57"/>
+      <c r="AG162" s="57"/>
+      <c r="AH162" s="57"/>
+      <c r="AI162" s="57"/>
+      <c r="AJ162" s="57"/>
+      <c r="AK162" s="57"/>
+      <c r="AL162" s="57"/>
+      <c r="AM162" s="57"/>
+      <c r="AN162" s="57"/>
+      <c r="AO162" s="57"/>
+      <c r="AP162" s="57"/>
+      <c r="AQ162" s="57"/>
+      <c r="AR162" s="57"/>
+      <c r="AS162" s="57"/>
+      <c r="AT162" s="57"/>
+      <c r="AU162" s="57"/>
+      <c r="AV162" s="89"/>
+    </row>
+    <row r="163" spans="2:48">
+      <c r="B163" s="88"/>
+      <c r="C163" s="57"/>
+      <c r="D163" s="57"/>
+      <c r="E163" s="57"/>
+      <c r="F163" s="57"/>
+      <c r="G163" s="57"/>
+      <c r="H163" s="57"/>
+      <c r="I163" s="57"/>
+      <c r="J163" s="57"/>
+      <c r="K163" s="57"/>
+      <c r="L163" s="57"/>
+      <c r="M163" s="57"/>
+      <c r="N163" s="57"/>
+      <c r="O163" s="57"/>
+      <c r="P163" s="57"/>
+      <c r="Q163" s="57"/>
+      <c r="R163" s="57"/>
+      <c r="S163" s="57"/>
+      <c r="T163" s="57"/>
+      <c r="U163" s="57"/>
+      <c r="V163" s="57"/>
+      <c r="W163" s="57"/>
+      <c r="X163" s="57"/>
+      <c r="Y163" s="57"/>
+      <c r="Z163" s="57"/>
+      <c r="AA163" s="57"/>
+      <c r="AB163" s="57"/>
+      <c r="AC163" s="57"/>
+      <c r="AD163" s="57"/>
+      <c r="AE163" s="57"/>
+      <c r="AF163" s="57"/>
+      <c r="AG163" s="57"/>
+      <c r="AH163" s="57"/>
+      <c r="AI163" s="57"/>
+      <c r="AJ163" s="57"/>
+      <c r="AK163" s="57"/>
+      <c r="AL163" s="57"/>
+      <c r="AM163" s="57"/>
+      <c r="AN163" s="57"/>
+      <c r="AO163" s="57"/>
+      <c r="AP163" s="57"/>
+      <c r="AQ163" s="57"/>
+      <c r="AR163" s="57"/>
+      <c r="AS163" s="57"/>
+      <c r="AT163" s="57"/>
+      <c r="AU163" s="57"/>
+      <c r="AV163" s="89"/>
+    </row>
+    <row r="164" spans="2:48" ht="14.4" thickBot="1">
+      <c r="B164" s="90"/>
+      <c r="C164" s="91"/>
+      <c r="D164" s="91"/>
+      <c r="E164" s="91"/>
+      <c r="F164" s="91"/>
+      <c r="G164" s="91"/>
+      <c r="H164" s="91"/>
+      <c r="I164" s="91"/>
+      <c r="J164" s="91"/>
+      <c r="K164" s="91"/>
+      <c r="L164" s="91"/>
+      <c r="M164" s="91"/>
+      <c r="N164" s="91"/>
+      <c r="O164" s="91"/>
+      <c r="P164" s="91"/>
+      <c r="Q164" s="91"/>
+      <c r="R164" s="91"/>
+      <c r="S164" s="91"/>
+      <c r="T164" s="91"/>
+      <c r="U164" s="91"/>
+      <c r="V164" s="91" t="s">
+        <v>87</v>
+      </c>
+      <c r="W164" s="91"/>
+      <c r="X164" s="91"/>
+      <c r="Y164" s="91"/>
+      <c r="Z164" s="91"/>
+      <c r="AA164" s="91"/>
+      <c r="AB164" s="91"/>
+      <c r="AC164" s="91"/>
+      <c r="AD164" s="91"/>
+      <c r="AE164" s="91"/>
+      <c r="AF164" s="91"/>
+      <c r="AG164" s="91"/>
+      <c r="AH164" s="91"/>
+      <c r="AI164" s="91"/>
+      <c r="AJ164" s="91"/>
+      <c r="AK164" s="91"/>
+      <c r="AL164" s="91"/>
+      <c r="AM164" s="91"/>
+      <c r="AN164" s="91"/>
+      <c r="AO164" s="91"/>
+      <c r="AP164" s="91"/>
+      <c r="AQ164" s="91"/>
+      <c r="AR164" s="91"/>
+      <c r="AS164" s="91"/>
+      <c r="AT164" s="91"/>
+      <c r="AU164" s="91"/>
+      <c r="AV164" s="92"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="21">
+    <mergeCell ref="T91:AB92"/>
+    <mergeCell ref="T100:AC102"/>
+    <mergeCell ref="T126:AB127"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="AO4:AR4"/>
     <mergeCell ref="AS4:AV4"/>
     <mergeCell ref="T76:AC78"/>
     <mergeCell ref="A1:C2"/>
@@ -10822,11 +12455,6 @@
     <mergeCell ref="AO3:AR3"/>
     <mergeCell ref="AS3:AV3"/>
     <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="T91:AB92"/>
-    <mergeCell ref="T100:AC102"/>
-    <mergeCell ref="T126:AB127"/>
-    <mergeCell ref="AK4:AN4"/>
-    <mergeCell ref="AO4:AR4"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.3" top="0.4" bottom="0.3" header="0.15" footer="0.15"/>
   <pageSetup paperSize="9" scale="51" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10856,12 +12484,12 @@
   <sheetData>
     <row r="1" spans="1:48">
       <c r="A1" s="215" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="216"/>
       <c r="C1" s="217"/>
       <c r="D1" s="215" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="216"/>
       <c r="F1" s="216"/>
@@ -10891,7 +12519,7 @@
       <c r="AD1" s="216"/>
       <c r="AE1" s="217"/>
       <c r="AF1" s="215" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AG1" s="216"/>
       <c r="AH1" s="216"/>
@@ -10943,7 +12571,7 @@
       <c r="AD2" s="219"/>
       <c r="AE2" s="220"/>
       <c r="AF2" s="209" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AG2" s="209"/>
       <c r="AH2" s="209"/>
@@ -10964,14 +12592,14 @@
     </row>
     <row r="3" spans="1:48">
       <c r="A3" s="221" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="221"/>
       <c r="C3" s="221"/>
       <c r="D3" s="221"/>
       <c r="E3" s="221"/>
       <c r="F3" s="222" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="222"/>
       <c r="H3" s="222"/>
@@ -10979,7 +12607,7 @@
       <c r="J3" s="222"/>
       <c r="K3" s="222"/>
       <c r="L3" s="221" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M3" s="221"/>
       <c r="N3" s="221"/>
@@ -10987,7 +12615,7 @@
       <c r="P3" s="221"/>
       <c r="Q3" s="221"/>
       <c r="R3" s="223" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S3" s="224"/>
       <c r="T3" s="224"/>
@@ -11003,7 +12631,7 @@
       <c r="AD3" s="224"/>
       <c r="AE3" s="225"/>
       <c r="AF3" s="226" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AG3" s="227"/>
       <c r="AH3" s="227"/>
@@ -11014,7 +12642,7 @@
       <c r="AM3" s="209"/>
       <c r="AN3" s="210"/>
       <c r="AO3" s="214" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AP3" s="209"/>
       <c r="AQ3" s="209"/>
@@ -11054,7 +12682,7 @@
       <c r="AD4" s="224"/>
       <c r="AE4" s="225"/>
       <c r="AF4" s="229" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG4" s="230"/>
       <c r="AH4" s="230"/>
@@ -11104,13 +12732,13 @@
   <sheetData>
     <row r="1" spans="1:47" ht="15" customHeight="1">
       <c r="A1" s="237" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="238"/>
       <c r="C1" s="238"/>
       <c r="D1" s="238"/>
       <c r="E1" s="241" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="242"/>
       <c r="G1" s="242"/>
@@ -11130,7 +12758,7 @@
       <c r="U1" s="242"/>
       <c r="V1" s="243"/>
       <c r="W1" s="247" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X1" s="248"/>
       <c r="Y1" s="248"/>
@@ -11169,26 +12797,26 @@
       <c r="T2" s="245"/>
       <c r="U2" s="245"/>
       <c r="V2" s="246"/>
-      <c r="W2" s="187" t="s">
-        <v>23</v>
+      <c r="W2" s="174" t="s">
+        <v>22</v>
       </c>
-      <c r="X2" s="188"/>
-      <c r="Y2" s="188"/>
-      <c r="Z2" s="188"/>
-      <c r="AA2" s="188"/>
-      <c r="AB2" s="188"/>
-      <c r="AC2" s="188"/>
-      <c r="AD2" s="188"/>
-      <c r="AE2" s="188"/>
-      <c r="AF2" s="188"/>
-      <c r="AG2" s="188"/>
-      <c r="AH2" s="188"/>
-      <c r="AI2" s="188"/>
-      <c r="AJ2" s="189"/>
+      <c r="X2" s="175"/>
+      <c r="Y2" s="175"/>
+      <c r="Z2" s="175"/>
+      <c r="AA2" s="175"/>
+      <c r="AB2" s="175"/>
+      <c r="AC2" s="175"/>
+      <c r="AD2" s="175"/>
+      <c r="AE2" s="175"/>
+      <c r="AF2" s="175"/>
+      <c r="AG2" s="175"/>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:47" ht="15" customHeight="1">
       <c r="A3" s="250" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="251"/>
       <c r="C3" s="251"/>
@@ -11198,7 +12826,7 @@
       <c r="G3" s="255"/>
       <c r="H3" s="256"/>
       <c r="I3" s="251" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="251"/>
       <c r="K3" s="251"/>
@@ -11214,7 +12842,7 @@
       <c r="U3" s="255"/>
       <c r="V3" s="263"/>
       <c r="W3" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X3" s="23"/>
       <c r="Y3" s="23"/>
@@ -11223,7 +12851,7 @@
       <c r="AB3" s="266"/>
       <c r="AC3" s="267"/>
       <c r="AD3" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE3" s="27"/>
       <c r="AF3" s="28"/>
@@ -11256,7 +12884,7 @@
       <c r="U4" s="258"/>
       <c r="V4" s="265"/>
       <c r="W4" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X4" s="24"/>
       <c r="Y4" s="24"/>
@@ -11265,7 +12893,7 @@
       <c r="AB4" s="232"/>
       <c r="AC4" s="233"/>
       <c r="AD4" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE4" s="29"/>
       <c r="AF4" s="30"/>
@@ -11279,7 +12907,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>

</xml_diff>